<commit_message>
EBEGU-409: Statistiken Gesuchsteller-Kinder-Betreuung implementieren inklusive Sichtbarkeit je Rolle
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -17,27 +17,6 @@
     <sheet name="Auszahlungen Periode" sheetId="8" r:id="rId8"/>
     <sheet name="Mitarbeiterinnen Jugendamt" sheetId="9" r:id="rId9"/>
   </sheets>
-  <definedNames>
-    <definedName name="angestellt">Data!$R$11</definedName>
-    <definedName name="anteilMonat">Data!$BM$11</definedName>
-    <definedName name="ausbildung">Data!$S$11</definedName>
-    <definedName name="bgPensum">Data!$BP$11</definedName>
-    <definedName name="geburtsdatum">Data!$AZ$11</definedName>
-    <definedName name="gesundheit">Data!$W$11</definedName>
-    <definedName name="gs2Angestellt">Data!$AH$11</definedName>
-    <definedName name="gs2Ausbildung">Data!$AI$11</definedName>
-    <definedName name="gs2Gesundheit">Data!$AM$11</definedName>
-    <definedName name="gs2Rav">Data!$AK$11</definedName>
-    <definedName name="gs2Selbstaendig">Data!$AJ$11</definedName>
-    <definedName name="gs2Zuschlag">Data!$AL$11</definedName>
-    <definedName name="nettotageIntervall">Data!$BL$11</definedName>
-    <definedName name="nettotageMonat">Data!$BK$11</definedName>
-    <definedName name="rav">Data!$U$11</definedName>
-    <definedName name="selbstaendig">Data!$T$11</definedName>
-    <definedName name="zeitabschnittBis">Data!$BJ$11</definedName>
-    <definedName name="zeitabschnittVon">Data!$BI$11</definedName>
-    <definedName name="zuschlag">Data!$V$11</definedName>
-  </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -48,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="230">
   <si>
     <t>Gesuche</t>
   </si>
@@ -461,9 +440,6 @@
     <t>Gesuchsteller-Kinder-Betreuung</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Zahlungsauftrag</t>
   </si>
   <si>
@@ -735,6 +711,12 @@
   </si>
   <si>
     <t>Ausblenden</t>
+  </si>
+  <si>
+    <t>Eingeschult</t>
+  </si>
+  <si>
+    <t>{eingeschult}</t>
   </si>
 </sst>
 </file>
@@ -944,7 +926,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1101,6 +1083,9 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1122,6 +1107,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1134,13 +1128,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1778,54 +1769,54 @@
       <c r="K6" s="17"/>
     </row>
     <row r="8" spans="1:25">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="70"/>
+      <c r="E8" s="71"/>
       <c r="F8" s="18"/>
-      <c r="G8" s="70" t="s">
+      <c r="G8" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="70"/>
-      <c r="N8" s="70"/>
-      <c r="O8" s="70"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="71"/>
       <c r="P8" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="70" t="s">
+      <c r="Q8" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="R8" s="70"/>
+      <c r="R8" s="71"/>
       <c r="S8" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="T8" s="70" t="s">
+      <c r="T8" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="U8" s="70"/>
-      <c r="V8" s="70"/>
-      <c r="W8" s="70"/>
-      <c r="X8" s="70"/>
-      <c r="Y8" s="70"/>
+      <c r="U8" s="71"/>
+      <c r="V8" s="71"/>
+      <c r="W8" s="71"/>
+      <c r="X8" s="71"/>
+      <c r="Y8" s="71"/>
     </row>
     <row r="9" spans="1:25">
-      <c r="A9" s="71"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="72"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="73"/>
       <c r="D9" s="21" t="s">
         <v>32</v>
       </c>
@@ -2207,79 +2198,79 @@
       <c r="G6" s="17"/>
     </row>
     <row r="8" spans="1:34" s="22" customFormat="1">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="71" t="s">
+      <c r="D8" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="71" t="s">
+      <c r="E8" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="71" t="s">
+      <c r="F8" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="71" t="s">
+      <c r="G8" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="70" t="s">
+      <c r="H8" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="70"/>
-      <c r="N8" s="70"/>
-      <c r="O8" s="70"/>
-      <c r="P8" s="70"/>
-      <c r="Q8" s="70"/>
-      <c r="R8" s="70"/>
-      <c r="S8" s="70"/>
-      <c r="T8" s="70" t="s">
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="71"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="U8" s="70"/>
-      <c r="V8" s="70" t="s">
+      <c r="U8" s="71"/>
+      <c r="V8" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="W8" s="70"/>
-      <c r="X8" s="70" t="s">
+      <c r="W8" s="71"/>
+      <c r="X8" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="Y8" s="70" t="s">
+      <c r="Y8" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="Z8" s="70" t="s">
+      <c r="Z8" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="AA8" s="70" t="s">
+      <c r="AA8" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="AB8" s="70"/>
-      <c r="AC8" s="70"/>
-      <c r="AD8" s="70"/>
-      <c r="AE8" s="70"/>
-      <c r="AF8" s="70" t="s">
+      <c r="AB8" s="71"/>
+      <c r="AC8" s="71"/>
+      <c r="AD8" s="71"/>
+      <c r="AE8" s="71"/>
+      <c r="AF8" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="AG8" s="70"/>
-      <c r="AH8" s="70"/>
+      <c r="AG8" s="71"/>
+      <c r="AH8" s="71"/>
     </row>
     <row r="9" spans="1:34">
-      <c r="A9" s="71"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
       <c r="H9" s="21" t="s">
         <v>60</v>
       </c>
@@ -2328,9 +2319,9 @@
       <c r="W9" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="X9" s="70"/>
-      <c r="Y9" s="70"/>
-      <c r="Z9" s="70"/>
+      <c r="X9" s="71"/>
+      <c r="Y9" s="71"/>
+      <c r="Z9" s="71"/>
       <c r="AA9" s="21" t="s">
         <v>72</v>
       </c>
@@ -2575,21 +2566,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="X8:X9"/>
+    <mergeCell ref="Y8:Y9"/>
+    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="AA8:AE8"/>
+    <mergeCell ref="AF8:AH8"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:S8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="V8:W8"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:S8"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:X9"/>
-    <mergeCell ref="Y8:Y9"/>
-    <mergeCell ref="Z8:Z9"/>
-    <mergeCell ref="AA8:AE8"/>
-    <mergeCell ref="AF8:AH8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2665,193 +2656,193 @@
       <c r="C4"/>
     </row>
     <row r="6" spans="1:46">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="71" t="s">
+      <c r="E6" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="71" t="s">
+      <c r="F6" s="72" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="70" t="s">
+      <c r="G6" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
-      <c r="O6" s="70"/>
-      <c r="P6" s="70"/>
-      <c r="Q6" s="70"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="70"/>
-      <c r="U6" s="70"/>
-      <c r="V6" s="70"/>
-      <c r="W6" s="70" t="s">
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="71"/>
+      <c r="P6" s="71"/>
+      <c r="Q6" s="71"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="71"/>
+      <c r="T6" s="71"/>
+      <c r="U6" s="71"/>
+      <c r="V6" s="71"/>
+      <c r="W6" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="X6" s="70"/>
-      <c r="Y6" s="70"/>
-      <c r="Z6" s="70"/>
-      <c r="AA6" s="70"/>
-      <c r="AB6" s="70"/>
-      <c r="AC6" s="70"/>
-      <c r="AD6" s="70"/>
-      <c r="AE6" s="70"/>
-      <c r="AF6" s="70"/>
-      <c r="AG6" s="70"/>
-      <c r="AH6" s="70"/>
-      <c r="AI6" s="70"/>
-      <c r="AJ6" s="70"/>
-      <c r="AK6" s="70"/>
-      <c r="AL6" s="70"/>
-      <c r="AM6" s="70" t="s">
+      <c r="X6" s="71"/>
+      <c r="Y6" s="71"/>
+      <c r="Z6" s="71"/>
+      <c r="AA6" s="71"/>
+      <c r="AB6" s="71"/>
+      <c r="AC6" s="71"/>
+      <c r="AD6" s="71"/>
+      <c r="AE6" s="71"/>
+      <c r="AF6" s="71"/>
+      <c r="AG6" s="71"/>
+      <c r="AH6" s="71"/>
+      <c r="AI6" s="71"/>
+      <c r="AJ6" s="71"/>
+      <c r="AK6" s="71"/>
+      <c r="AL6" s="71"/>
+      <c r="AM6" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="AN6" s="70"/>
-      <c r="AO6" s="70" t="s">
+      <c r="AN6" s="71"/>
+      <c r="AO6" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="AP6" s="70"/>
-      <c r="AQ6" s="70"/>
-      <c r="AR6" s="70"/>
-      <c r="AS6" s="70" t="s">
+      <c r="AP6" s="71"/>
+      <c r="AQ6" s="71"/>
+      <c r="AR6" s="71"/>
+      <c r="AS6" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="AT6" s="70" t="s">
+      <c r="AT6" s="71" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:46">
-      <c r="A7" s="71"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="70" t="s">
+      <c r="A7" s="72"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="70" t="s">
+      <c r="H7" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="70" t="s">
+      <c r="I7" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="70" t="s">
+      <c r="J7" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="K7" s="70" t="s">
+      <c r="K7" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="L7" s="70" t="s">
+      <c r="L7" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="M7" s="70" t="s">
+      <c r="M7" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="N7" s="70" t="s">
+      <c r="N7" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="O7" s="70" t="s">
+      <c r="O7" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="P7" s="73" t="s">
+      <c r="P7" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="73"/>
-      <c r="S7" s="73"/>
-      <c r="T7" s="73"/>
-      <c r="U7" s="73"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="74"/>
       <c r="V7" s="27"/>
-      <c r="W7" s="70" t="s">
+      <c r="W7" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="X7" s="70" t="s">
+      <c r="X7" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="Y7" s="70" t="s">
+      <c r="Y7" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="Z7" s="70" t="s">
+      <c r="Z7" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="AA7" s="70" t="s">
+      <c r="AA7" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="AB7" s="70" t="s">
+      <c r="AB7" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="AC7" s="70" t="s">
+      <c r="AC7" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="AD7" s="70" t="s">
+      <c r="AD7" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="AE7" s="70" t="s">
+      <c r="AE7" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="AF7" s="73" t="s">
+      <c r="AF7" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="AG7" s="73"/>
-      <c r="AH7" s="73"/>
-      <c r="AI7" s="73"/>
-      <c r="AJ7" s="73"/>
-      <c r="AK7" s="73"/>
+      <c r="AG7" s="74"/>
+      <c r="AH7" s="74"/>
+      <c r="AI7" s="74"/>
+      <c r="AJ7" s="74"/>
+      <c r="AK7" s="74"/>
       <c r="AL7" s="27"/>
-      <c r="AM7" s="70" t="s">
+      <c r="AM7" s="71" t="s">
         <v>98</v>
       </c>
-      <c r="AN7" s="74" t="s">
+      <c r="AN7" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="AO7" s="70" t="s">
+      <c r="AO7" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="AP7" s="70" t="s">
+      <c r="AP7" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="AQ7" s="70" t="s">
+      <c r="AQ7" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="AR7" s="70" t="s">
+      <c r="AR7" s="71" t="s">
         <v>103</v>
       </c>
-      <c r="AS7" s="70"/>
-      <c r="AT7" s="70"/>
+      <c r="AS7" s="71"/>
+      <c r="AT7" s="71"/>
     </row>
     <row r="8" spans="1:46">
-      <c r="A8" s="71"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="70"/>
-      <c r="N8" s="70"/>
-      <c r="O8" s="70"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="71"/>
       <c r="P8" s="23" t="s">
         <v>32</v>
       </c>
@@ -2873,15 +2864,15 @@
       <c r="V8" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="W8" s="70"/>
-      <c r="X8" s="70"/>
-      <c r="Y8" s="70"/>
-      <c r="Z8" s="70"/>
-      <c r="AA8" s="70"/>
-      <c r="AB8" s="70"/>
-      <c r="AC8" s="70"/>
-      <c r="AD8" s="70"/>
-      <c r="AE8" s="70"/>
+      <c r="W8" s="71"/>
+      <c r="X8" s="71"/>
+      <c r="Y8" s="71"/>
+      <c r="Z8" s="71"/>
+      <c r="AA8" s="71"/>
+      <c r="AB8" s="71"/>
+      <c r="AC8" s="71"/>
+      <c r="AD8" s="71"/>
+      <c r="AE8" s="71"/>
       <c r="AF8" s="23" t="s">
         <v>32</v>
       </c>
@@ -2903,14 +2894,14 @@
       <c r="AL8" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="AM8" s="70"/>
-      <c r="AN8" s="74"/>
-      <c r="AO8" s="70"/>
-      <c r="AP8" s="70"/>
-      <c r="AQ8" s="70"/>
-      <c r="AR8" s="70"/>
-      <c r="AS8" s="70"/>
-      <c r="AT8" s="70"/>
+      <c r="AM8" s="71"/>
+      <c r="AN8" s="75"/>
+      <c r="AO8" s="71"/>
+      <c r="AP8" s="71"/>
+      <c r="AQ8" s="71"/>
+      <c r="AR8" s="71"/>
+      <c r="AS8" s="71"/>
+      <c r="AT8" s="71"/>
     </row>
     <row r="9" spans="1:46" s="30" customFormat="1">
       <c r="A9" s="28" t="s">
@@ -3176,6 +3167,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="AQ7:AQ8"/>
+    <mergeCell ref="AS6:AS8"/>
+    <mergeCell ref="AT6:AT8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:U7"/>
+    <mergeCell ref="W7:W8"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="AF7:AK7"/>
+    <mergeCell ref="AM7:AM8"/>
+    <mergeCell ref="AN7:AN8"/>
+    <mergeCell ref="AO7:AO8"/>
+    <mergeCell ref="AE7:AE8"/>
+    <mergeCell ref="Z7:Z8"/>
     <mergeCell ref="AP7:AP8"/>
     <mergeCell ref="AR7:AR8"/>
     <mergeCell ref="A6:A8"/>
@@ -3192,28 +3205,6 @@
     <mergeCell ref="AB7:AB8"/>
     <mergeCell ref="AC7:AC8"/>
     <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="AF7:AK7"/>
-    <mergeCell ref="AM7:AM8"/>
-    <mergeCell ref="AN7:AN8"/>
-    <mergeCell ref="AO7:AO8"/>
-    <mergeCell ref="AE7:AE8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AQ7:AQ8"/>
-    <mergeCell ref="AS6:AS8"/>
-    <mergeCell ref="AT6:AT8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:U7"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="X7:X8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3332,64 +3323,64 @@
       <c r="M5"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="72" t="s">
+      <c r="D7" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="72" t="s">
+      <c r="E7" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="72" t="s">
+      <c r="F7" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="71" t="s">
+      <c r="G7" s="72" t="s">
         <v>74</v>
       </c>
-      <c r="H7" s="72" t="s">
+      <c r="H7" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="I7" s="72" t="s">
+      <c r="I7" s="73" t="s">
         <v>115</v>
       </c>
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
       <c r="L7" s="31"/>
-      <c r="M7" s="76" t="s">
+      <c r="M7" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="N7" s="75" t="s">
+      <c r="N7" s="76" t="s">
         <v>117</v>
       </c>
-      <c r="O7" s="75"/>
-      <c r="P7" s="75"/>
-      <c r="Q7" s="71" t="s">
+      <c r="O7" s="76"/>
+      <c r="P7" s="76"/>
+      <c r="Q7" s="72" t="s">
         <v>118</v>
       </c>
-      <c r="R7" s="71" t="s">
+      <c r="R7" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="S7" s="71" t="s">
+      <c r="S7" s="72" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="71"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
       <c r="J8" s="8" t="s">
         <v>120</v>
       </c>
@@ -3399,7 +3390,7 @@
       <c r="L8" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="76"/>
+      <c r="M8" s="77"/>
       <c r="N8" s="32" t="s">
         <v>77</v>
       </c>
@@ -3409,9 +3400,9 @@
       <c r="P8" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="Q8" s="71"/>
-      <c r="R8" s="71"/>
-      <c r="S8" s="71"/>
+      <c r="Q8" s="72"/>
+      <c r="R8" s="72"/>
+      <c r="S8" s="72"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="33" t="s">
@@ -4081,11 +4072,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
     <mergeCell ref="N7:P7"/>
     <mergeCell ref="Q7:Q8"/>
     <mergeCell ref="R7:R8"/>
@@ -4095,6 +4081,11 @@
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="M7:M8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4106,10 +4097,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BV26"/>
+  <dimension ref="A1:BW26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BJ11" sqref="BJ11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BS12" sqref="BS12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4134,18 +4125,22 @@
     <col min="50" max="52" width="12.7109375"/>
     <col min="53" max="53" width="16.7109375"/>
     <col min="54" max="55" width="12.7109375"/>
-    <col min="56" max="60" width="22"/>
-    <col min="61" max="62" width="12.7109375"/>
-    <col min="65" max="66" width="12.7109375"/>
-    <col min="67" max="67" width="16.85546875"/>
-    <col min="68" max="68" width="12.7109375"/>
-    <col min="69" max="69" width="19.42578125"/>
-    <col min="70" max="70" width="16.85546875"/>
-    <col min="71" max="73" width="12.7109375"/>
-    <col min="74" max="1028" width="10.5703125"/>
+    <col min="56" max="56" width="22"/>
+    <col min="57" max="57" width="10.85546875" customWidth="1"/>
+    <col min="58" max="61" width="22"/>
+    <col min="62" max="63" width="12.7109375"/>
+    <col min="64" max="64" width="11.28515625" customWidth="1"/>
+    <col min="65" max="65" width="16" customWidth="1"/>
+    <col min="66" max="67" width="12.7109375"/>
+    <col min="68" max="68" width="16.85546875"/>
+    <col min="69" max="69" width="12.7109375"/>
+    <col min="70" max="70" width="19.42578125"/>
+    <col min="71" max="71" width="16.85546875"/>
+    <col min="72" max="74" width="12.7109375"/>
+    <col min="75" max="1029" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" ht="21">
+    <row r="1" spans="1:75" ht="21">
       <c r="A1" s="2" t="s">
         <v>136</v>
       </c>
@@ -4156,10 +4151,10 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:74">
+    <row r="2" spans="1:75">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:74">
+    <row r="3" spans="1:75">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -4169,326 +4164,330 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="BK3" s="69" t="s">
-        <v>228</v>
-      </c>
-      <c r="BL3" s="69"/>
-    </row>
-    <row r="4" spans="1:74">
+      <c r="BL3" s="69" t="s">
+        <v>227</v>
+      </c>
+      <c r="BM3" s="69"/>
+    </row>
+    <row r="4" spans="1:75">
       <c r="A4" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:74">
+    <row r="5" spans="1:75">
       <c r="A5" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:74">
+    <row r="6" spans="1:75">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
     </row>
-    <row r="8" spans="1:74" s="22" customFormat="1">
-      <c r="A8" s="71" t="s">
+    <row r="8" spans="1:75" s="22" customFormat="1">
+      <c r="A8" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="71" t="s">
+      <c r="D8" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="71" t="s">
+      <c r="E8" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="71" t="s">
+      <c r="F8" s="72" t="s">
         <v>85</v>
       </c>
-      <c r="G8" s="71" t="s">
+      <c r="G8" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="70" t="s">
+      <c r="H8" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="70"/>
-      <c r="N8" s="70"/>
-      <c r="O8" s="70"/>
-      <c r="P8" s="70"/>
-      <c r="Q8" s="83"/>
-      <c r="R8" s="83"/>
-      <c r="S8" s="83"/>
-      <c r="T8" s="83"/>
-      <c r="U8" s="83"/>
-      <c r="V8" s="83"/>
-      <c r="W8" s="83"/>
-      <c r="X8" s="70" t="s">
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="71"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="78"/>
+      <c r="S8" s="78"/>
+      <c r="T8" s="78"/>
+      <c r="U8" s="78"/>
+      <c r="V8" s="78"/>
+      <c r="W8" s="78"/>
+      <c r="X8" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="Y8" s="70"/>
-      <c r="Z8" s="70"/>
-      <c r="AA8" s="70"/>
-      <c r="AB8" s="70"/>
-      <c r="AC8" s="70"/>
-      <c r="AD8" s="70"/>
-      <c r="AE8" s="70"/>
-      <c r="AF8" s="70"/>
-      <c r="AG8" s="83"/>
-      <c r="AH8" s="83"/>
-      <c r="AI8" s="83"/>
-      <c r="AJ8" s="83"/>
-      <c r="AK8" s="83"/>
-      <c r="AL8" s="83"/>
-      <c r="AM8" s="83"/>
-      <c r="AN8" s="75" t="s">
+      <c r="Y8" s="71"/>
+      <c r="Z8" s="71"/>
+      <c r="AA8" s="71"/>
+      <c r="AB8" s="71"/>
+      <c r="AC8" s="71"/>
+      <c r="AD8" s="71"/>
+      <c r="AE8" s="71"/>
+      <c r="AF8" s="71"/>
+      <c r="AG8" s="78"/>
+      <c r="AH8" s="78"/>
+      <c r="AI8" s="78"/>
+      <c r="AJ8" s="78"/>
+      <c r="AK8" s="78"/>
+      <c r="AL8" s="78"/>
+      <c r="AM8" s="78"/>
+      <c r="AN8" s="76" t="s">
         <v>86</v>
       </c>
-      <c r="AO8" s="75"/>
-      <c r="AP8" s="75"/>
-      <c r="AQ8" s="75" t="s">
+      <c r="AO8" s="76"/>
+      <c r="AP8" s="76"/>
+      <c r="AQ8" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="AR8" s="75"/>
-      <c r="AS8" s="75"/>
-      <c r="AT8" s="75"/>
-      <c r="AU8" s="75"/>
-      <c r="AV8" s="75" t="s">
+      <c r="AR8" s="76"/>
+      <c r="AS8" s="76"/>
+      <c r="AT8" s="76"/>
+      <c r="AU8" s="76"/>
+      <c r="AV8" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="AW8" s="70" t="s">
+      <c r="AW8" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="AX8" s="70" t="s">
+      <c r="AX8" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="AY8" s="70"/>
-      <c r="AZ8" s="70"/>
-      <c r="BA8" s="70"/>
-      <c r="BB8" s="70"/>
+      <c r="AY8" s="71"/>
+      <c r="AZ8" s="71"/>
+      <c r="BA8" s="71"/>
+      <c r="BB8" s="71"/>
       <c r="BC8" s="18"/>
       <c r="BD8" s="18"/>
-      <c r="BE8" s="18"/>
+      <c r="BE8" s="70"/>
       <c r="BF8" s="18"/>
       <c r="BG8" s="18"/>
       <c r="BH8" s="18"/>
-      <c r="BI8" s="70" t="s">
+      <c r="BI8" s="18"/>
+      <c r="BJ8" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="BJ8" s="70"/>
-      <c r="BK8" s="70"/>
-      <c r="BL8" s="70"/>
-      <c r="BM8" s="70"/>
-      <c r="BN8" s="70"/>
-      <c r="BO8" s="70"/>
-      <c r="BP8" s="70"/>
-      <c r="BQ8" s="70"/>
-      <c r="BR8" s="70"/>
-      <c r="BS8" s="70"/>
-      <c r="BT8" s="70"/>
-      <c r="BU8" s="70"/>
-    </row>
-    <row r="9" spans="1:74">
-      <c r="A9" s="71"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="70" t="s">
+      <c r="BK8" s="71"/>
+      <c r="BL8" s="71"/>
+      <c r="BM8" s="71"/>
+      <c r="BN8" s="71"/>
+      <c r="BO8" s="71"/>
+      <c r="BP8" s="71"/>
+      <c r="BQ8" s="71"/>
+      <c r="BR8" s="71"/>
+      <c r="BS8" s="71"/>
+      <c r="BT8" s="71"/>
+      <c r="BU8" s="71"/>
+      <c r="BV8" s="71"/>
+    </row>
+    <row r="9" spans="1:75">
+      <c r="A9" s="72"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="70" t="s">
+      <c r="I9" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="J9" s="70" t="s">
+      <c r="J9" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="K9" s="70" t="s">
+      <c r="K9" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="L9" s="70" t="s">
+      <c r="L9" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="M9" s="70" t="s">
+      <c r="M9" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="N9" s="70" t="s">
+      <c r="N9" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="O9" s="70" t="s">
+      <c r="O9" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="P9" s="81" t="s">
+      <c r="P9" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="Q9" s="81" t="s">
+      <c r="Q9" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="R9" s="73"/>
-      <c r="S9" s="73"/>
-      <c r="T9" s="73"/>
-      <c r="U9" s="73"/>
-      <c r="V9" s="73"/>
+      <c r="R9" s="74"/>
+      <c r="S9" s="74"/>
+      <c r="T9" s="74"/>
+      <c r="U9" s="74"/>
+      <c r="V9" s="74"/>
       <c r="W9" s="27"/>
-      <c r="X9" s="74" t="s">
+      <c r="X9" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="Y9" s="70" t="s">
+      <c r="Y9" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="Z9" s="70" t="s">
+      <c r="Z9" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="AA9" s="70" t="s">
+      <c r="AA9" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="AB9" s="70" t="s">
+      <c r="AB9" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="AC9" s="70" t="s">
+      <c r="AC9" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="AD9" s="70" t="s">
+      <c r="AD9" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="AE9" s="70" t="s">
+      <c r="AE9" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="AF9" s="81" t="s">
+      <c r="AF9" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="AG9" s="81" t="s">
+      <c r="AG9" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="AH9" s="73"/>
-      <c r="AI9" s="73"/>
-      <c r="AJ9" s="73"/>
-      <c r="AK9" s="73"/>
-      <c r="AL9" s="73"/>
+      <c r="AH9" s="74"/>
+      <c r="AI9" s="74"/>
+      <c r="AJ9" s="74"/>
+      <c r="AK9" s="74"/>
+      <c r="AL9" s="74"/>
       <c r="AM9" s="27"/>
-      <c r="AN9" s="77" t="s">
+      <c r="AN9" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="AO9" s="79" t="s">
-        <v>198</v>
-      </c>
-      <c r="AP9" s="75" t="s">
+      <c r="AO9" s="83" t="s">
+        <v>197</v>
+      </c>
+      <c r="AP9" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="AQ9" s="79" t="s">
-        <v>223</v>
-      </c>
-      <c r="AR9" s="79" t="s">
-        <v>225</v>
-      </c>
-      <c r="AS9" s="75" t="s">
+      <c r="AQ9" s="83" t="s">
+        <v>222</v>
+      </c>
+      <c r="AR9" s="83" t="s">
+        <v>224</v>
+      </c>
+      <c r="AS9" s="76" t="s">
         <v>101</v>
       </c>
-      <c r="AT9" s="78" t="s">
-        <v>202</v>
-      </c>
-      <c r="AU9" s="75" t="s">
+      <c r="AT9" s="82" t="s">
+        <v>201</v>
+      </c>
+      <c r="AU9" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="AV9" s="75"/>
-      <c r="AW9" s="70"/>
-      <c r="AX9" s="70" t="s">
+      <c r="AV9" s="76"/>
+      <c r="AW9" s="71"/>
+      <c r="AX9" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="AY9" s="70" t="s">
+      <c r="AY9" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="AZ9" s="70" t="s">
+      <c r="AZ9" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="BA9" s="82" t="s">
-        <v>210</v>
-      </c>
-      <c r="BB9" s="70" t="s">
+      <c r="BA9" s="80" t="s">
+        <v>209</v>
+      </c>
+      <c r="BB9" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="BC9" s="70" t="s">
+      <c r="BC9" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="BD9" s="70" t="s">
+      <c r="BD9" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="BE9" s="70" t="s">
+      <c r="BE9" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="BF9" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="BF9" s="70" t="s">
+      <c r="BG9" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="BG9" s="70" t="s">
+      <c r="BH9" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="BH9" s="70" t="s">
+      <c r="BI9" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="BI9" s="70" t="s">
+      <c r="BJ9" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="BJ9" s="70" t="s">
+      <c r="BK9" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="BK9" s="66"/>
       <c r="BL9" s="66"/>
-      <c r="BM9" s="70" t="s">
+      <c r="BM9" s="66"/>
+      <c r="BN9" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="BN9" s="70" t="s">
+      <c r="BO9" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="BO9" s="70"/>
-      <c r="BP9" s="70"/>
-      <c r="BQ9" s="70"/>
-      <c r="BR9" s="70"/>
-      <c r="BS9" s="70" t="s">
+      <c r="BP9" s="71"/>
+      <c r="BQ9" s="71"/>
+      <c r="BR9" s="71"/>
+      <c r="BS9" s="71"/>
+      <c r="BT9" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="BT9" s="70"/>
-      <c r="BU9" s="70"/>
-    </row>
-    <row r="10" spans="1:74">
-      <c r="A10" s="71"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="70"/>
-      <c r="M10" s="70"/>
-      <c r="N10" s="70"/>
-      <c r="O10" s="70"/>
-      <c r="P10" s="70"/>
+      <c r="BU9" s="71"/>
+      <c r="BV9" s="71"/>
+    </row>
+    <row r="10" spans="1:75">
+      <c r="A10" s="72"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="71"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="71"/>
       <c r="Q10" s="56" t="s">
         <v>32</v>
       </c>
@@ -4508,17 +4507,17 @@
         <v>108</v>
       </c>
       <c r="W10" s="57" t="s">
-        <v>181</v>
-      </c>
-      <c r="X10" s="70"/>
-      <c r="Y10" s="70"/>
-      <c r="Z10" s="70"/>
-      <c r="AA10" s="70"/>
-      <c r="AB10" s="70"/>
-      <c r="AC10" s="70"/>
-      <c r="AD10" s="70"/>
-      <c r="AE10" s="70"/>
-      <c r="AF10" s="70"/>
+        <v>180</v>
+      </c>
+      <c r="X10" s="71"/>
+      <c r="Y10" s="71"/>
+      <c r="Z10" s="71"/>
+      <c r="AA10" s="71"/>
+      <c r="AB10" s="71"/>
+      <c r="AC10" s="71"/>
+      <c r="AD10" s="71"/>
+      <c r="AE10" s="71"/>
+      <c r="AF10" s="71"/>
       <c r="AG10" s="56" t="s">
         <v>32</v>
       </c>
@@ -4538,296 +4537,303 @@
         <v>108</v>
       </c>
       <c r="AM10" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="AN10" s="76"/>
+      <c r="AO10" s="84"/>
+      <c r="AP10" s="76"/>
+      <c r="AQ10" s="84"/>
+      <c r="AR10" s="84"/>
+      <c r="AS10" s="76"/>
+      <c r="AT10" s="76"/>
+      <c r="AU10" s="76"/>
+      <c r="AV10" s="76"/>
+      <c r="AW10" s="71"/>
+      <c r="AX10" s="71"/>
+      <c r="AY10" s="71"/>
+      <c r="AZ10" s="71"/>
+      <c r="BA10" s="71"/>
+      <c r="BB10" s="71"/>
+      <c r="BC10" s="71"/>
+      <c r="BD10" s="71"/>
+      <c r="BE10" s="85"/>
+      <c r="BF10" s="71"/>
+      <c r="BG10" s="71"/>
+      <c r="BH10" s="71"/>
+      <c r="BI10" s="71"/>
+      <c r="BJ10" s="71"/>
+      <c r="BK10" s="71"/>
+      <c r="BL10" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="BM10" s="67" t="s">
+        <v>121</v>
+      </c>
+      <c r="BN10" s="71"/>
+      <c r="BO10" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="BP10" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="BQ10" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="BR10" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="BS10" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="BT10" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="BU10" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="BV10" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:75">
+      <c r="A11" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="F11" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="I11" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="J11" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="K11" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="L11" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="M11" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="N11" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="O11" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="P11" s="54" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q11" s="55" t="e">
+        <f>R11+S11+T11+U11+V11+W11</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R11" s="54" t="s">
+        <v>174</v>
+      </c>
+      <c r="S11" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="T11" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="U11" s="54" t="s">
+        <v>177</v>
+      </c>
+      <c r="V11" s="54" t="s">
+        <v>178</v>
+      </c>
+      <c r="W11" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="X11" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="AN10" s="75"/>
-      <c r="AO10" s="80"/>
-      <c r="AP10" s="75"/>
-      <c r="AQ10" s="80"/>
-      <c r="AR10" s="80"/>
-      <c r="AS10" s="75"/>
-      <c r="AT10" s="75"/>
-      <c r="AU10" s="75"/>
-      <c r="AV10" s="75"/>
-      <c r="AW10" s="70"/>
-      <c r="AX10" s="70"/>
-      <c r="AY10" s="70"/>
-      <c r="AZ10" s="70"/>
-      <c r="BA10" s="70"/>
-      <c r="BB10" s="70"/>
-      <c r="BC10" s="70"/>
-      <c r="BD10" s="70"/>
-      <c r="BE10" s="70"/>
-      <c r="BF10" s="70"/>
-      <c r="BG10" s="70"/>
-      <c r="BH10" s="70"/>
-      <c r="BI10" s="70"/>
-      <c r="BJ10" s="70"/>
-      <c r="BK10" s="66" t="s">
-        <v>120</v>
-      </c>
-      <c r="BL10" s="67" t="s">
-        <v>121</v>
-      </c>
-      <c r="BM10" s="70"/>
-      <c r="BN10" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="BO10" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="BP10" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="BQ10" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="BR10" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="BS10" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="BT10" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="BU10" s="21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:74">
-      <c r="A11" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="B11" s="54" t="s">
-        <v>161</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="D11" s="54" t="s">
-        <v>163</v>
-      </c>
-      <c r="E11" s="54" t="s">
-        <v>164</v>
-      </c>
-      <c r="F11" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="G11" s="54" t="s">
-        <v>159</v>
-      </c>
-      <c r="H11" s="54" t="s">
-        <v>166</v>
-      </c>
-      <c r="I11" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="J11" s="54" t="s">
-        <v>168</v>
-      </c>
-      <c r="K11" s="54" t="s">
-        <v>169</v>
-      </c>
-      <c r="L11" s="54" t="s">
-        <v>170</v>
-      </c>
-      <c r="M11" s="54" t="s">
-        <v>171</v>
-      </c>
-      <c r="N11" s="54" t="s">
-        <v>172</v>
-      </c>
-      <c r="O11" s="54" t="s">
-        <v>173</v>
-      </c>
-      <c r="P11" s="54" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q11" s="55" t="e">
-        <f>angestellt+ausbildung+selbstaendig+rav+zuschlag+gesundheit</f>
+      <c r="Y11" s="54" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z11" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA11" s="54" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB11" s="54" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC11" s="54" t="s">
+        <v>186</v>
+      </c>
+      <c r="AD11" s="54" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE11" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="AF11" s="54" t="s">
+        <v>189</v>
+      </c>
+      <c r="AG11" s="58" t="e">
+        <f>AH11+AI11+AJ11+AK11+AL11+AM11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R11" s="54" t="s">
-        <v>175</v>
-      </c>
-      <c r="S11" s="54" t="s">
-        <v>176</v>
-      </c>
-      <c r="T11" s="54" t="s">
-        <v>177</v>
-      </c>
-      <c r="U11" s="54" t="s">
-        <v>178</v>
-      </c>
-      <c r="V11" s="54" t="s">
-        <v>179</v>
-      </c>
-      <c r="W11" s="54" t="s">
-        <v>180</v>
-      </c>
-      <c r="X11" s="54" t="s">
-        <v>182</v>
-      </c>
-      <c r="Y11" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z11" s="54" t="s">
-        <v>184</v>
-      </c>
-      <c r="AA11" s="54" t="s">
-        <v>185</v>
-      </c>
-      <c r="AB11" s="54" t="s">
-        <v>186</v>
-      </c>
-      <c r="AC11" s="54" t="s">
-        <v>187</v>
-      </c>
-      <c r="AD11" s="54" t="s">
-        <v>188</v>
-      </c>
-      <c r="AE11" s="54" t="s">
-        <v>189</v>
-      </c>
-      <c r="AF11" s="54" t="s">
+      <c r="AH11" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="AG11" s="58" t="e">
-        <f>gs2Angestellt+gs2Ausbildung+gs2Selbstaendig+gs2Rav+gs2Zuschlag+gs2Gesundheit</f>
+      <c r="AI11" s="54" t="s">
+        <v>191</v>
+      </c>
+      <c r="AJ11" s="54" t="s">
+        <v>192</v>
+      </c>
+      <c r="AK11" s="54" t="s">
+        <v>193</v>
+      </c>
+      <c r="AL11" s="54" t="s">
+        <v>194</v>
+      </c>
+      <c r="AM11" s="54" t="s">
+        <v>195</v>
+      </c>
+      <c r="AN11" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="AO11" s="54" t="s">
+        <v>198</v>
+      </c>
+      <c r="AP11" s="54" t="s">
+        <v>199</v>
+      </c>
+      <c r="AQ11" s="54" t="s">
+        <v>223</v>
+      </c>
+      <c r="AR11" s="54" t="s">
+        <v>225</v>
+      </c>
+      <c r="AS11" s="54" t="s">
+        <v>226</v>
+      </c>
+      <c r="AT11" s="54" t="s">
+        <v>200</v>
+      </c>
+      <c r="AU11" s="54" t="s">
+        <v>202</v>
+      </c>
+      <c r="AV11" s="54" t="s">
+        <v>203</v>
+      </c>
+      <c r="AW11" s="54" t="s">
+        <v>204</v>
+      </c>
+      <c r="AX11" s="60" t="s">
+        <v>205</v>
+      </c>
+      <c r="AY11" s="60" t="s">
+        <v>206</v>
+      </c>
+      <c r="AZ11" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="BA11" s="60" t="s">
+        <v>208</v>
+      </c>
+      <c r="BB11" s="61" t="e">
+        <f>IF(BJ11&lt;=EOMONTH(AZ11,12),"Ja","Nein")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AH11" s="54" t="s">
-        <v>191</v>
-      </c>
-      <c r="AI11" s="54" t="s">
-        <v>192</v>
-      </c>
-      <c r="AJ11" s="54" t="s">
-        <v>193</v>
-      </c>
-      <c r="AK11" s="54" t="s">
-        <v>194</v>
-      </c>
-      <c r="AL11" s="54" t="s">
-        <v>195</v>
-      </c>
-      <c r="AM11" s="54" t="s">
-        <v>196</v>
-      </c>
-      <c r="AN11" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="AO11" s="54" t="s">
-        <v>199</v>
-      </c>
-      <c r="AP11" s="54" t="s">
-        <v>200</v>
-      </c>
-      <c r="AQ11" s="54" t="s">
-        <v>224</v>
-      </c>
-      <c r="AR11" s="54" t="s">
-        <v>226</v>
-      </c>
-      <c r="AS11" s="54" t="s">
-        <v>227</v>
-      </c>
-      <c r="AT11" s="54" t="s">
-        <v>201</v>
-      </c>
-      <c r="AU11" s="54" t="s">
-        <v>203</v>
-      </c>
-      <c r="AV11" s="54" t="s">
-        <v>204</v>
-      </c>
-      <c r="AW11" s="54" t="s">
-        <v>205</v>
-      </c>
-      <c r="AX11" s="60" t="s">
-        <v>206</v>
-      </c>
-      <c r="AY11" s="60" t="s">
-        <v>207</v>
-      </c>
-      <c r="AZ11" s="60" t="s">
-        <v>208</v>
-      </c>
-      <c r="BA11" s="60" t="s">
-        <v>209</v>
-      </c>
-      <c r="BB11" s="61" t="e">
-        <f>IF(zeitabschnittVon&gt;EOMONTH(geburtsdatum,12),"Nein","Ja")</f>
+      <c r="BC11" s="60" t="s">
+        <v>211</v>
+      </c>
+      <c r="BD11" s="60" t="s">
+        <v>210</v>
+      </c>
+      <c r="BE11" s="60" t="s">
+        <v>229</v>
+      </c>
+      <c r="BF11" s="61" t="e">
+        <f>IF(BJ11&lt;=EOMONTH(AZ11,12),"Ja","Nein")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BC11" s="60" t="s">
+      <c r="BG11" s="61" t="e">
+        <f>IF(AND(BJ11&gt;=EOMONTH(AZ11,13),BJ11&lt;=EOMONTH(AZ11,48)),"Ja","Nein")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BH11" s="61" t="e">
+        <f>IF(AND(BJ11&gt;=EOMONTH(AZ11,48),BJ11&lt;=EOMONTH(AZ11,72)),"Ja","Nein")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BI11" s="61" t="e">
+        <f>IF(BJ11&gt;=EOMONTH(AZ11,73),"Ja","Nein")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BJ11" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="BD11" s="60" t="s">
-        <v>211</v>
-      </c>
-      <c r="BE11" s="61" t="e">
-        <f>IF(zeitabschnittVon&gt;EOMONTH(geburtsdatum,12),"Nein","Ja")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BF11" s="61" t="s">
-        <v>137</v>
-      </c>
-      <c r="BG11" s="61" t="s">
-        <v>137</v>
-      </c>
-      <c r="BH11" s="61" t="s">
-        <v>137</v>
-      </c>
-      <c r="BI11" s="63" t="s">
+      <c r="BK11" s="63" t="s">
         <v>213</v>
       </c>
-      <c r="BJ11" s="63" t="s">
+      <c r="BL11" s="63" t="e">
+        <f>NETWORKDAYS((zeitabschnittVon-DAY(zeitabschnittVon)+1),(EOMONTH(zeitabschnittVon,0)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="BM11" s="63" t="e">
+        <f>NETWORKDAYS(zeitabschnittVon,zeitabschnittBis)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="BN11" s="61" t="e">
+        <f>BM11/BL11</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="BO11" s="60" t="s">
         <v>214</v>
       </c>
-      <c r="BK11" s="63" t="e">
-        <f>NETWORKDAYS((zeitabschnittVon-DAY(zeitabschnittVon)+1),(EOMONTH(zeitabschnittVon,0)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BL11" s="63" t="e">
-        <f>NETWORKDAYS(zeitabschnittVon,zeitabschnittBis)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BM11" s="61" t="e">
-        <f>nettotageIntervall/nettotageMonat</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BN11" s="60" t="s">
+      <c r="BP11" s="60" t="s">
         <v>215</v>
       </c>
-      <c r="BO11" s="60" t="s">
+      <c r="BQ11" s="60" t="s">
         <v>216</v>
       </c>
-      <c r="BP11" s="60" t="s">
+      <c r="BR11" s="60" t="s">
         <v>217</v>
       </c>
-      <c r="BQ11" s="60" t="s">
+      <c r="BS11" s="61" t="e">
+        <f>BN11/BQ11</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="BT11" s="64" t="s">
         <v>218</v>
       </c>
-      <c r="BR11" s="61" t="e">
-        <f>anteilMonat/bgPensum</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BS11" s="64" t="s">
+      <c r="BU11" s="64" t="s">
         <v>219</v>
       </c>
-      <c r="BT11" s="64" t="s">
+      <c r="BV11" s="65" t="s">
         <v>220</v>
       </c>
-      <c r="BU11" s="65" t="s">
+      <c r="BW11" s="62" t="s">
         <v>221</v>
       </c>
-      <c r="BV11" s="62" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="12" spans="1:74">
+    </row>
+    <row r="12" spans="1:75">
       <c r="A12" s="13" t="s">
         <v>81</v>
       </c>
@@ -4890,15 +4896,15 @@
       <c r="BB12" s="13"/>
       <c r="BC12" s="13"/>
       <c r="BD12" s="13"/>
-      <c r="BE12" s="13"/>
+      <c r="BE12" s="47"/>
       <c r="BF12" s="13"/>
       <c r="BG12" s="13"/>
       <c r="BH12" s="13"/>
       <c r="BI12" s="13"/>
       <c r="BJ12" s="13"/>
-      <c r="BK12" s="47"/>
+      <c r="BK12" s="13"/>
       <c r="BL12" s="47"/>
-      <c r="BM12" s="13"/>
+      <c r="BM12" s="47"/>
       <c r="BN12" s="13"/>
       <c r="BO12" s="13"/>
       <c r="BP12" s="13"/>
@@ -4907,8 +4913,9 @@
       <c r="BS12" s="13"/>
       <c r="BT12" s="13"/>
       <c r="BU12" s="13"/>
-    </row>
-    <row r="13" spans="1:74">
+      <c r="BV12" s="13"/>
+    </row>
+    <row r="13" spans="1:75">
       <c r="A13" s="13" t="s">
         <v>82</v>
       </c>
@@ -4971,15 +4978,15 @@
       <c r="BB13" s="13"/>
       <c r="BC13" s="13"/>
       <c r="BD13" s="13"/>
-      <c r="BE13" s="13"/>
+      <c r="BE13" s="47"/>
       <c r="BF13" s="13"/>
       <c r="BG13" s="13"/>
       <c r="BH13" s="13"/>
       <c r="BI13" s="13"/>
       <c r="BJ13" s="13"/>
-      <c r="BK13" s="47"/>
+      <c r="BK13" s="13"/>
       <c r="BL13" s="47"/>
-      <c r="BM13" s="13"/>
+      <c r="BM13" s="47"/>
       <c r="BN13" s="13"/>
       <c r="BO13" s="13"/>
       <c r="BP13" s="13"/>
@@ -4988,8 +4995,9 @@
       <c r="BS13" s="13"/>
       <c r="BT13" s="13"/>
       <c r="BU13" s="13"/>
-    </row>
-    <row r="14" spans="1:74">
+      <c r="BV13" s="13"/>
+    </row>
+    <row r="14" spans="1:75">
       <c r="A14" s="47" t="s">
         <v>17</v>
       </c>
@@ -5052,15 +5060,15 @@
       <c r="BB14" s="13"/>
       <c r="BC14" s="13"/>
       <c r="BD14" s="13"/>
-      <c r="BE14" s="13"/>
+      <c r="BE14" s="47"/>
       <c r="BF14" s="13"/>
       <c r="BG14" s="13"/>
       <c r="BH14" s="13"/>
       <c r="BI14" s="13"/>
       <c r="BJ14" s="13"/>
-      <c r="BK14" s="47"/>
+      <c r="BK14" s="13"/>
       <c r="BL14" s="47"/>
-      <c r="BM14" s="13"/>
+      <c r="BM14" s="47"/>
       <c r="BN14" s="13"/>
       <c r="BO14" s="13"/>
       <c r="BP14" s="13"/>
@@ -5069,13 +5077,14 @@
       <c r="BS14" s="13"/>
       <c r="BT14" s="13"/>
       <c r="BU14" s="13"/>
-    </row>
-    <row r="15" spans="1:74">
+      <c r="BV14" s="13"/>
+    </row>
+    <row r="15" spans="1:75">
       <c r="A15" s="26"/>
       <c r="B15" s="26"/>
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:74">
+    <row r="16" spans="1:75">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
@@ -5086,97 +5095,131 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:61">
+    <row r="17" spans="1:62">
       <c r="A17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:61">
+    <row r="18" spans="1:62">
       <c r="A18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:61">
+    <row r="19" spans="1:62">
       <c r="A19" t="s">
         <v>22</v>
       </c>
       <c r="AZ19" s="7">
         <v>42216</v>
       </c>
-      <c r="BE19" t="str">
-        <f>IF(BI19&lt;=EOMONTH(AZ19,12),"JA","NEIN")</f>
+      <c r="BF19" t="str">
+        <f>IF(BJ19&lt;=EOMONTH(AZ19,12),"JA","NEIN")</f>
         <v>NEIN</v>
       </c>
-      <c r="BF19" t="str">
-        <f>IF(AND(BI19&gt;=EOMONTH(AZ19,13),BI19&lt;=EOMONTH(AZ19,48)),"JA","NEIN")</f>
+      <c r="BG19" t="str">
+        <f>IF(AND(BJ19&gt;=EOMONTH(AZ19,13),BJ19&lt;=EOMONTH(AZ19,48)),"JA","NEIN")</f>
         <v>JA</v>
       </c>
-      <c r="BG19" t="str">
-        <f>IF(AND(BI19&gt;=EOMONTH(AZ19,48),BI19&lt;=EOMONTH(AZ19,72)),"JA","NEIN")</f>
-        <v>NEIN</v>
-      </c>
       <c r="BH19" t="str">
-        <f>IF(BI19&gt;=EOMONTH(AZ19,73),"JA","NEIN")</f>
-        <v>NEIN</v>
-      </c>
-      <c r="BI19" s="7">
+        <f>IF(AND(BJ19&gt;=EOMONTH(AZ19,48),BJ19&lt;=EOMONTH(AZ19,72)),"Ja","Nein")</f>
+        <v>Nein</v>
+      </c>
+      <c r="BI19" t="str">
+        <f>IF(BJ19&gt;=EOMONTH(AZ19,73),"Ja","Nein")</f>
+        <v>Nein</v>
+      </c>
+      <c r="BJ19" s="7">
         <v>42948</v>
       </c>
     </row>
-    <row r="21" spans="1:61">
-      <c r="BE21" s="68">
+    <row r="21" spans="1:62">
+      <c r="BF21" s="68">
         <f>EOMONTH(AZ19,12)</f>
         <v>42582</v>
       </c>
-      <c r="BF21" t="b">
-        <f>AND(BI19&gt;EOMONTH(AZ19,13),BI19&lt;EOMONTH(AZ19,48))</f>
+      <c r="BG21" t="b">
+        <f>AND(BJ19&gt;EOMONTH(AZ19,13),BJ19&lt;EOMONTH(AZ19,48))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:61">
-      <c r="BF22" t="b">
-        <f>BI19&gt;EOMONTH(AZ19,13)</f>
+    <row r="22" spans="1:62">
+      <c r="BG22" t="b">
+        <f>BJ19&gt;EOMONTH(AZ19,13)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:61">
-      <c r="BF23" t="b">
-        <f>BI19&lt;EOMONTH(AZ19,48)</f>
+    <row r="23" spans="1:62">
+      <c r="BG23" t="b">
+        <f>BJ19&lt;EOMONTH(AZ19,48)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:61">
-      <c r="BF25" s="68">
+    <row r="25" spans="1:62">
+      <c r="BG25" s="68">
         <f>EOMONTH(AZ19,13)</f>
         <v>42613</v>
       </c>
-      <c r="BG25" s="68">
+      <c r="BH25" s="68">
         <f>EOMONTH(AZ19,48)</f>
         <v>43677</v>
       </c>
-      <c r="BH25" s="68">
+      <c r="BI25" s="68">
         <f>EOMONTH(AZ19,73)</f>
         <v>44439</v>
       </c>
     </row>
-    <row r="26" spans="1:61">
-      <c r="BF26" s="68">
+    <row r="26" spans="1:62">
+      <c r="BG26" s="68">
         <f>EOMONTH(AZ19,47)</f>
         <v>43646</v>
       </c>
-      <c r="BG26" s="68">
+      <c r="BH26" s="68">
         <f>EOMONTH(AZ19,72)</f>
         <v>44408</v>
       </c>
-      <c r="BH26" s="68"/>
+      <c r="BI26" s="68"/>
     </row>
   </sheetData>
-  <mergeCells count="59">
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
+  <mergeCells count="60">
+    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BJ9:BJ10"/>
+    <mergeCell ref="BK9:BK10"/>
+    <mergeCell ref="BN9:BN10"/>
+    <mergeCell ref="BO9:BS9"/>
+    <mergeCell ref="AN9:AN10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AU10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AL9"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AQ8:AU8"/>
+    <mergeCell ref="AV8:AV10"/>
+    <mergeCell ref="AW8:AW10"/>
+    <mergeCell ref="AX8:BB8"/>
+    <mergeCell ref="BJ8:BV8"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="AZ9:AZ10"/>
+    <mergeCell ref="BA9:BA10"/>
+    <mergeCell ref="BB9:BB10"/>
+    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="BD9:BD10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="BT9:BV9"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="G8:G10"/>
     <mergeCell ref="H8:W8"/>
@@ -5193,44 +5236,11 @@
     <mergeCell ref="P9:P10"/>
     <mergeCell ref="Q9:V9"/>
     <mergeCell ref="X9:X10"/>
-    <mergeCell ref="AQ8:AU8"/>
-    <mergeCell ref="AV8:AV10"/>
-    <mergeCell ref="AW8:AW10"/>
-    <mergeCell ref="AX8:BB8"/>
-    <mergeCell ref="BI8:BU8"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="AZ9:AZ10"/>
-    <mergeCell ref="BA9:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BC9:BC10"/>
-    <mergeCell ref="BD9:BD10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BS9:BU9"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AL9"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AN9:AN10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AT9:AT10"/>
-    <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BJ9:BJ10"/>
-    <mergeCell ref="BM9:BM10"/>
-    <mergeCell ref="BN9:BR9"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -5260,7 +5270,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21">
       <c r="A1" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" s="2"/>
       <c r="G1"/>
@@ -5288,10 +5298,10 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>139</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>140</v>
       </c>
       <c r="G4"/>
       <c r="H4"/>
@@ -5306,7 +5316,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>60</v>
@@ -5327,15 +5337,15 @@
         <v>74</v>
       </c>
       <c r="J6" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="K6" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>11</v>
@@ -5365,12 +5375,12 @@
         <v>1338.2</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>11</v>
@@ -5400,18 +5410,18 @@
         <v>121.65</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" s="49" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D9" s="50" t="s">
         <v>128</v>
@@ -5435,18 +5445,18 @@
         <v>-121.65</v>
       </c>
       <c r="K9" s="49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B10" s="49" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D10" s="50" t="s">
         <v>128</v>
@@ -5470,18 +5480,18 @@
         <v>-425.8</v>
       </c>
       <c r="K10" s="49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B11" s="49" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D11" s="50" t="s">
         <v>128</v>
@@ -5505,7 +5515,7 @@
         <v>669.1</v>
       </c>
       <c r="K11" s="49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -5560,7 +5570,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21">
       <c r="A1" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1"/>
@@ -5582,15 +5592,15 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" s="24">
         <v>42597</v>
@@ -5601,7 +5611,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" s="24">
         <v>42628</v>
@@ -5612,7 +5622,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B8" s="24">
         <v>42597</v>
@@ -5623,7 +5633,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B9" s="24">
         <v>42628</v>
@@ -5680,7 +5690,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21">
       <c r="A1" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -5723,18 +5733,18 @@
         <v>61</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>152</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>154</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>155</v>
       </c>
       <c r="C8" s="14">
         <v>725</v>

</xml_diff>

<commit_message>
EBEGU-406 / EBEGU-409: Adressen, Zivilstand und Erwerbspensen nach Stichtag
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -425,7 +425,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -645,7 +645,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -654,11 +654,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -666,33 +666,32 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -714,6 +713,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1082,8 +1082,8 @@
   </sheetPr>
   <dimension ref="A1:BW23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG11" sqref="AG11"/>
+    <sheetView tabSelected="1" topLeftCell="BE1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BT25" sqref="BT25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1147,8 +1147,8 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="BL3" s="39"/>
-      <c r="BM3" s="39"/>
+      <c r="BL3" s="38"/>
+      <c r="BM3" s="38"/>
     </row>
     <row r="4" spans="1:75">
       <c r="A4" t="s">
@@ -1181,88 +1181,88 @@
       <c r="F6" s="10"/>
     </row>
     <row r="8" spans="1:75" s="13" customFormat="1">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="42" t="s">
+      <c r="G8" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
-      <c r="T8" s="47"/>
-      <c r="U8" s="47"/>
-      <c r="V8" s="47"/>
-      <c r="W8" s="47"/>
-      <c r="X8" s="41" t="s">
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="43"/>
+      <c r="W8" s="43"/>
+      <c r="X8" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="41"/>
-      <c r="AB8" s="41"/>
-      <c r="AC8" s="41"/>
-      <c r="AD8" s="41"/>
-      <c r="AE8" s="41"/>
-      <c r="AF8" s="41"/>
-      <c r="AG8" s="47"/>
-      <c r="AH8" s="47"/>
-      <c r="AI8" s="47"/>
-      <c r="AJ8" s="47"/>
-      <c r="AK8" s="47"/>
-      <c r="AL8" s="47"/>
-      <c r="AM8" s="47"/>
-      <c r="AN8" s="46" t="s">
+      <c r="Y8" s="42"/>
+      <c r="Z8" s="42"/>
+      <c r="AA8" s="42"/>
+      <c r="AB8" s="42"/>
+      <c r="AC8" s="42"/>
+      <c r="AD8" s="42"/>
+      <c r="AE8" s="42"/>
+      <c r="AF8" s="42"/>
+      <c r="AG8" s="43"/>
+      <c r="AH8" s="43"/>
+      <c r="AI8" s="43"/>
+      <c r="AJ8" s="43"/>
+      <c r="AK8" s="43"/>
+      <c r="AL8" s="43"/>
+      <c r="AM8" s="43"/>
+      <c r="AN8" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="AO8" s="46"/>
-      <c r="AP8" s="46"/>
-      <c r="AQ8" s="46" t="s">
+      <c r="AO8" s="44"/>
+      <c r="AP8" s="44"/>
+      <c r="AQ8" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="AR8" s="46"/>
-      <c r="AS8" s="46"/>
-      <c r="AT8" s="46"/>
-      <c r="AU8" s="46"/>
-      <c r="AV8" s="46" t="s">
+      <c r="AR8" s="44"/>
+      <c r="AS8" s="44"/>
+      <c r="AT8" s="44"/>
+      <c r="AU8" s="44"/>
+      <c r="AV8" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="AW8" s="41" t="s">
+      <c r="AW8" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="AX8" s="41" t="s">
+      <c r="AX8" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="AY8" s="41"/>
-      <c r="AZ8" s="41"/>
-      <c r="BA8" s="41"/>
-      <c r="BB8" s="41"/>
+      <c r="AY8" s="42"/>
+      <c r="AZ8" s="42"/>
+      <c r="BA8" s="42"/>
+      <c r="BB8" s="42"/>
       <c r="BC8" s="11"/>
       <c r="BD8" s="11"/>
       <c r="BE8" s="29"/>
@@ -1270,205 +1270,205 @@
       <c r="BG8" s="11"/>
       <c r="BH8" s="11"/>
       <c r="BI8" s="11"/>
-      <c r="BJ8" s="41" t="s">
+      <c r="BJ8" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="BK8" s="41"/>
-      <c r="BL8" s="41"/>
-      <c r="BM8" s="41"/>
-      <c r="BN8" s="41"/>
-      <c r="BO8" s="41"/>
-      <c r="BP8" s="41"/>
-      <c r="BQ8" s="41"/>
-      <c r="BR8" s="41"/>
-      <c r="BS8" s="41"/>
-      <c r="BT8" s="41"/>
-      <c r="BU8" s="41"/>
-      <c r="BV8" s="41"/>
+      <c r="BK8" s="42"/>
+      <c r="BL8" s="42"/>
+      <c r="BM8" s="42"/>
+      <c r="BN8" s="42"/>
+      <c r="BO8" s="42"/>
+      <c r="BP8" s="42"/>
+      <c r="BQ8" s="42"/>
+      <c r="BR8" s="42"/>
+      <c r="BS8" s="42"/>
+      <c r="BT8" s="42"/>
+      <c r="BU8" s="42"/>
+      <c r="BV8" s="42"/>
     </row>
     <row r="9" spans="1:75">
-      <c r="A9" s="42"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="41" t="s">
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="41" t="s">
+      <c r="J9" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="L9" s="41" t="s">
+      <c r="L9" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="M9" s="41" t="s">
+      <c r="M9" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="N9" s="41" t="s">
+      <c r="N9" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="41" t="s">
+      <c r="O9" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="48" t="s">
+      <c r="P9" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="Q9" s="48" t="s">
+      <c r="Q9" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="R9" s="44"/>
-      <c r="S9" s="44"/>
-      <c r="T9" s="44"/>
-      <c r="U9" s="44"/>
-      <c r="V9" s="44"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="46"/>
+      <c r="V9" s="46"/>
       <c r="W9" s="15"/>
-      <c r="X9" s="45" t="s">
+      <c r="X9" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="Y9" s="41" t="s">
+      <c r="Y9" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="Z9" s="41" t="s">
+      <c r="Z9" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="AA9" s="41" t="s">
+      <c r="AA9" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="AB9" s="41" t="s">
+      <c r="AB9" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="AC9" s="41" t="s">
+      <c r="AC9" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="AD9" s="41" t="s">
+      <c r="AD9" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="AE9" s="41" t="s">
+      <c r="AE9" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="AF9" s="48" t="s">
+      <c r="AF9" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="AG9" s="48" t="s">
+      <c r="AG9" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="AH9" s="44"/>
-      <c r="AI9" s="44"/>
-      <c r="AJ9" s="44"/>
-      <c r="AK9" s="44"/>
-      <c r="AL9" s="44"/>
+      <c r="AH9" s="46"/>
+      <c r="AI9" s="46"/>
+      <c r="AJ9" s="46"/>
+      <c r="AK9" s="46"/>
+      <c r="AL9" s="46"/>
       <c r="AM9" s="15"/>
-      <c r="AN9" s="50" t="s">
+      <c r="AN9" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="AO9" s="52" t="s">
+      <c r="AO9" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="AP9" s="46" t="s">
+      <c r="AP9" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="AQ9" s="52" t="s">
+      <c r="AQ9" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="AR9" s="52" t="s">
+      <c r="AR9" s="51" t="s">
         <v>128</v>
       </c>
-      <c r="AS9" s="46" t="s">
+      <c r="AS9" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="AT9" s="51" t="s">
+      <c r="AT9" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="AU9" s="46" t="s">
+      <c r="AU9" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="AV9" s="46"/>
-      <c r="AW9" s="41"/>
-      <c r="AX9" s="41" t="s">
+      <c r="AV9" s="44"/>
+      <c r="AW9" s="42"/>
+      <c r="AX9" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="AY9" s="41" t="s">
+      <c r="AY9" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="AZ9" s="41" t="s">
+      <c r="AZ9" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="BA9" s="49" t="s">
+      <c r="BA9" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="BB9" s="41" t="s">
+      <c r="BB9" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="BC9" s="41" t="s">
+      <c r="BC9" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="BD9" s="41" t="s">
+      <c r="BD9" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="BE9" s="54" t="s">
+      <c r="BE9" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="BF9" s="41" t="s">
+      <c r="BF9" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BG9" s="41" t="s">
+      <c r="BG9" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="BH9" s="41" t="s">
+      <c r="BH9" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="BI9" s="41" t="s">
+      <c r="BI9" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="BJ9" s="41" t="s">
+      <c r="BJ9" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="BK9" s="41" t="s">
+      <c r="BK9" s="42" t="s">
         <v>5</v>
       </c>
       <c r="BL9" s="26"/>
       <c r="BM9" s="26"/>
-      <c r="BN9" s="41" t="s">
+      <c r="BN9" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="BO9" s="41" t="s">
+      <c r="BO9" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="BP9" s="41"/>
-      <c r="BQ9" s="41"/>
-      <c r="BR9" s="41"/>
-      <c r="BS9" s="41"/>
-      <c r="BT9" s="41" t="s">
+      <c r="BP9" s="42"/>
+      <c r="BQ9" s="42"/>
+      <c r="BR9" s="42"/>
+      <c r="BS9" s="42"/>
+      <c r="BT9" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="BU9" s="41"/>
-      <c r="BV9" s="41"/>
+      <c r="BU9" s="42"/>
+      <c r="BV9" s="42"/>
     </row>
     <row r="10" spans="1:75">
-      <c r="A10" s="42"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="41"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="42"/>
       <c r="Q10" s="18" t="s">
         <v>6</v>
       </c>
@@ -1490,15 +1490,15 @@
       <c r="W10" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="X10" s="41"/>
-      <c r="Y10" s="41"/>
-      <c r="Z10" s="41"/>
-      <c r="AA10" s="41"/>
-      <c r="AB10" s="41"/>
-      <c r="AC10" s="41"/>
-      <c r="AD10" s="41"/>
-      <c r="AE10" s="41"/>
-      <c r="AF10" s="41"/>
+      <c r="X10" s="42"/>
+      <c r="Y10" s="42"/>
+      <c r="Z10" s="42"/>
+      <c r="AA10" s="42"/>
+      <c r="AB10" s="42"/>
+      <c r="AC10" s="42"/>
+      <c r="AD10" s="42"/>
+      <c r="AE10" s="42"/>
+      <c r="AF10" s="42"/>
       <c r="AG10" s="18" t="s">
         <v>6</v>
       </c>
@@ -1520,37 +1520,37 @@
       <c r="AM10" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="AN10" s="46"/>
-      <c r="AO10" s="53"/>
-      <c r="AP10" s="46"/>
-      <c r="AQ10" s="53"/>
-      <c r="AR10" s="53"/>
-      <c r="AS10" s="46"/>
-      <c r="AT10" s="46"/>
-      <c r="AU10" s="46"/>
-      <c r="AV10" s="46"/>
-      <c r="AW10" s="41"/>
-      <c r="AX10" s="41"/>
-      <c r="AY10" s="41"/>
-      <c r="AZ10" s="41"/>
-      <c r="BA10" s="41"/>
-      <c r="BB10" s="41"/>
-      <c r="BC10" s="41"/>
-      <c r="BD10" s="41"/>
-      <c r="BE10" s="55"/>
-      <c r="BF10" s="41"/>
-      <c r="BG10" s="41"/>
-      <c r="BH10" s="41"/>
-      <c r="BI10" s="41"/>
-      <c r="BJ10" s="41"/>
-      <c r="BK10" s="41"/>
+      <c r="AN10" s="44"/>
+      <c r="AO10" s="52"/>
+      <c r="AP10" s="44"/>
+      <c r="AQ10" s="52"/>
+      <c r="AR10" s="52"/>
+      <c r="AS10" s="44"/>
+      <c r="AT10" s="44"/>
+      <c r="AU10" s="44"/>
+      <c r="AV10" s="44"/>
+      <c r="AW10" s="42"/>
+      <c r="AX10" s="42"/>
+      <c r="AY10" s="42"/>
+      <c r="AZ10" s="42"/>
+      <c r="BA10" s="42"/>
+      <c r="BB10" s="42"/>
+      <c r="BC10" s="42"/>
+      <c r="BD10" s="42"/>
+      <c r="BE10" s="54"/>
+      <c r="BF10" s="42"/>
+      <c r="BG10" s="42"/>
+      <c r="BH10" s="42"/>
+      <c r="BI10" s="42"/>
+      <c r="BJ10" s="42"/>
+      <c r="BK10" s="42"/>
       <c r="BL10" s="26" t="s">
         <v>56</v>
       </c>
       <c r="BM10" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="BN10" s="41"/>
+      <c r="BN10" s="42"/>
       <c r="BO10" s="12" t="s">
         <v>26</v>
       </c>
@@ -1781,7 +1781,7 @@
         <f>NETWORKDAYS(BJ11,BK11)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BN11" s="40" t="e">
+      <c r="BN11" s="39" t="e">
         <f>BM11/BL11</f>
         <v>#VALUE!</v>
       </c>
@@ -1797,8 +1797,8 @@
       <c r="BR11" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="BS11" s="38" t="e">
-        <f>IF(BQ11&gt;0,BN11/BQ11,0)</f>
+      <c r="BS11" s="55" t="e">
+        <f>BQ11*BN11</f>
         <v>#VALUE!</v>
       </c>
       <c r="BT11" s="24" t="s">

</xml_diff>

<commit_message>
EBEGU-407: Statistiken Gesuchsteller implementieren inklusive Sichtbarkeit je Rolle. Anpassungen Excels und Sortierung
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -484,7 +484,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -579,23 +579,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -644,7 +633,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -669,51 +657,51 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1080,10 +1068,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BW23"/>
+  <dimension ref="A1:BX23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BT25" sqref="BT25"/>
+    <sheetView tabSelected="1" topLeftCell="BF1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BN11" sqref="BN11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1120,10 +1108,11 @@
     <col min="70" max="70" width="19.42578125"/>
     <col min="71" max="71" width="16.85546875"/>
     <col min="72" max="74" width="12.7109375"/>
-    <col min="75" max="1029" width="10.5703125"/>
+    <col min="75" max="75" width="13.42578125" customWidth="1"/>
+    <col min="76" max="1029" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="21">
+    <row r="1" spans="1:76" ht="21">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -1134,10 +1123,10 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:75">
+    <row r="2" spans="1:76">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:75">
+    <row r="3" spans="1:76">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1147,10 +1136,10 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="BL3" s="38"/>
-      <c r="BM3" s="38"/>
+      <c r="BL3" s="37"/>
+      <c r="BM3" s="37"/>
     </row>
-    <row r="4" spans="1:75">
+    <row r="4" spans="1:76">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1159,7 +1148,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:75">
+    <row r="5" spans="1:76">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1168,7 +1157,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:75">
+    <row r="6" spans="1:76">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1180,295 +1169,295 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
     </row>
-    <row r="8" spans="1:75" s="13" customFormat="1">
-      <c r="A8" s="40" t="s">
+    <row r="8" spans="1:76" s="13" customFormat="1">
+      <c r="A8" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="40" t="s">
+      <c r="G8" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="42" t="s">
+      <c r="H8" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="43"/>
-      <c r="S8" s="43"/>
-      <c r="T8" s="43"/>
-      <c r="U8" s="43"/>
-      <c r="V8" s="43"/>
-      <c r="W8" s="43"/>
-      <c r="X8" s="42" t="s">
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="51"/>
+      <c r="V8" s="51"/>
+      <c r="W8" s="51"/>
+      <c r="X8" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="Y8" s="42"/>
-      <c r="Z8" s="42"/>
-      <c r="AA8" s="42"/>
-      <c r="AB8" s="42"/>
-      <c r="AC8" s="42"/>
-      <c r="AD8" s="42"/>
-      <c r="AE8" s="42"/>
-      <c r="AF8" s="42"/>
-      <c r="AG8" s="43"/>
-      <c r="AH8" s="43"/>
-      <c r="AI8" s="43"/>
-      <c r="AJ8" s="43"/>
-      <c r="AK8" s="43"/>
-      <c r="AL8" s="43"/>
-      <c r="AM8" s="43"/>
-      <c r="AN8" s="44" t="s">
+      <c r="Y8" s="39"/>
+      <c r="Z8" s="39"/>
+      <c r="AA8" s="39"/>
+      <c r="AB8" s="39"/>
+      <c r="AC8" s="39"/>
+      <c r="AD8" s="39"/>
+      <c r="AE8" s="39"/>
+      <c r="AF8" s="39"/>
+      <c r="AG8" s="51"/>
+      <c r="AH8" s="51"/>
+      <c r="AI8" s="51"/>
+      <c r="AJ8" s="51"/>
+      <c r="AK8" s="51"/>
+      <c r="AL8" s="51"/>
+      <c r="AM8" s="51"/>
+      <c r="AN8" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="AO8" s="44"/>
-      <c r="AP8" s="44"/>
-      <c r="AQ8" s="44" t="s">
+      <c r="AO8" s="41"/>
+      <c r="AP8" s="41"/>
+      <c r="AQ8" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="AR8" s="44"/>
-      <c r="AS8" s="44"/>
-      <c r="AT8" s="44"/>
-      <c r="AU8" s="44"/>
-      <c r="AV8" s="44" t="s">
+      <c r="AR8" s="41"/>
+      <c r="AS8" s="41"/>
+      <c r="AT8" s="41"/>
+      <c r="AU8" s="41"/>
+      <c r="AV8" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="AW8" s="42" t="s">
+      <c r="AW8" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="AX8" s="42" t="s">
+      <c r="AX8" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AY8" s="42"/>
-      <c r="AZ8" s="42"/>
-      <c r="BA8" s="42"/>
-      <c r="BB8" s="42"/>
+      <c r="AY8" s="39"/>
+      <c r="AZ8" s="39"/>
+      <c r="BA8" s="39"/>
+      <c r="BB8" s="39"/>
       <c r="BC8" s="11"/>
       <c r="BD8" s="11"/>
-      <c r="BE8" s="29"/>
+      <c r="BE8" s="28"/>
       <c r="BF8" s="11"/>
       <c r="BG8" s="11"/>
       <c r="BH8" s="11"/>
       <c r="BI8" s="11"/>
-      <c r="BJ8" s="42" t="s">
+      <c r="BJ8" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="BK8" s="42"/>
-      <c r="BL8" s="42"/>
-      <c r="BM8" s="42"/>
-      <c r="BN8" s="42"/>
-      <c r="BO8" s="42"/>
-      <c r="BP8" s="42"/>
-      <c r="BQ8" s="42"/>
-      <c r="BR8" s="42"/>
-      <c r="BS8" s="42"/>
-      <c r="BT8" s="42"/>
-      <c r="BU8" s="42"/>
-      <c r="BV8" s="42"/>
+      <c r="BK8" s="39"/>
+      <c r="BL8" s="39"/>
+      <c r="BM8" s="39"/>
+      <c r="BN8" s="39"/>
+      <c r="BO8" s="39"/>
+      <c r="BP8" s="39"/>
+      <c r="BQ8" s="39"/>
+      <c r="BR8" s="39"/>
+      <c r="BS8" s="39"/>
+      <c r="BT8" s="39"/>
+      <c r="BU8" s="39"/>
+      <c r="BV8" s="39"/>
     </row>
-    <row r="9" spans="1:75">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="42" t="s">
+    <row r="9" spans="1:76">
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="42" t="s">
+      <c r="J9" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="K9" s="42" t="s">
+      <c r="K9" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="L9" s="42" t="s">
+      <c r="L9" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="M9" s="42" t="s">
+      <c r="M9" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="N9" s="42" t="s">
+      <c r="N9" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="42" t="s">
+      <c r="O9" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="45" t="s">
+      <c r="P9" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="Q9" s="45" t="s">
+      <c r="Q9" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="R9" s="46"/>
-      <c r="S9" s="46"/>
-      <c r="T9" s="46"/>
-      <c r="U9" s="46"/>
-      <c r="V9" s="46"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="48"/>
+      <c r="U9" s="48"/>
+      <c r="V9" s="48"/>
       <c r="W9" s="15"/>
-      <c r="X9" s="47" t="s">
+      <c r="X9" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="Y9" s="42" t="s">
+      <c r="Y9" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="Z9" s="42" t="s">
+      <c r="Z9" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="AA9" s="42" t="s">
+      <c r="AA9" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="AB9" s="42" t="s">
+      <c r="AB9" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="AC9" s="42" t="s">
+      <c r="AC9" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="AD9" s="42" t="s">
+      <c r="AD9" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="AE9" s="42" t="s">
+      <c r="AE9" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="AF9" s="45" t="s">
+      <c r="AF9" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="AG9" s="45" t="s">
+      <c r="AG9" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="AH9" s="46"/>
-      <c r="AI9" s="46"/>
-      <c r="AJ9" s="46"/>
-      <c r="AK9" s="46"/>
-      <c r="AL9" s="46"/>
+      <c r="AH9" s="48"/>
+      <c r="AI9" s="48"/>
+      <c r="AJ9" s="48"/>
+      <c r="AK9" s="48"/>
+      <c r="AL9" s="48"/>
       <c r="AM9" s="15"/>
-      <c r="AN9" s="49" t="s">
+      <c r="AN9" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="AO9" s="51" t="s">
+      <c r="AO9" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="AP9" s="44" t="s">
+      <c r="AP9" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="AQ9" s="51" t="s">
+      <c r="AQ9" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="AR9" s="51" t="s">
+      <c r="AR9" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="AS9" s="44" t="s">
+      <c r="AS9" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="AT9" s="50" t="s">
+      <c r="AT9" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="AU9" s="44" t="s">
+      <c r="AU9" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="AV9" s="44"/>
-      <c r="AW9" s="42"/>
-      <c r="AX9" s="42" t="s">
+      <c r="AV9" s="41"/>
+      <c r="AW9" s="39"/>
+      <c r="AX9" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="AY9" s="42" t="s">
+      <c r="AY9" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="AZ9" s="42" t="s">
+      <c r="AZ9" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="BA9" s="48" t="s">
+      <c r="BA9" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="BB9" s="42" t="s">
+      <c r="BB9" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="BC9" s="42" t="s">
+      <c r="BC9" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="BD9" s="42" t="s">
+      <c r="BD9" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="BE9" s="53" t="s">
+      <c r="BE9" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="BF9" s="42" t="s">
+      <c r="BF9" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="BG9" s="42" t="s">
+      <c r="BG9" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="BH9" s="42" t="s">
+      <c r="BH9" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="BI9" s="42" t="s">
+      <c r="BI9" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="BJ9" s="42" t="s">
+      <c r="BJ9" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="BK9" s="42" t="s">
+      <c r="BK9" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="BL9" s="26"/>
-      <c r="BM9" s="26"/>
-      <c r="BN9" s="42" t="s">
+      <c r="BL9" s="25"/>
+      <c r="BM9" s="25"/>
+      <c r="BN9" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="BO9" s="42" t="s">
+      <c r="BO9" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="BP9" s="42"/>
-      <c r="BQ9" s="42"/>
-      <c r="BR9" s="42"/>
-      <c r="BS9" s="42"/>
-      <c r="BT9" s="42" t="s">
+      <c r="BP9" s="39"/>
+      <c r="BQ9" s="39"/>
+      <c r="BR9" s="39"/>
+      <c r="BS9" s="39"/>
+      <c r="BT9" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="BU9" s="42"/>
-      <c r="BV9" s="42"/>
+      <c r="BU9" s="39"/>
+      <c r="BV9" s="39"/>
     </row>
-    <row r="10" spans="1:75">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
+    <row r="10" spans="1:76">
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
       <c r="Q10" s="18" t="s">
         <v>6</v>
       </c>
@@ -1490,15 +1479,15 @@
       <c r="W10" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="X10" s="42"/>
-      <c r="Y10" s="42"/>
-      <c r="Z10" s="42"/>
-      <c r="AA10" s="42"/>
-      <c r="AB10" s="42"/>
-      <c r="AC10" s="42"/>
-      <c r="AD10" s="42"/>
-      <c r="AE10" s="42"/>
-      <c r="AF10" s="42"/>
+      <c r="X10" s="39"/>
+      <c r="Y10" s="39"/>
+      <c r="Z10" s="39"/>
+      <c r="AA10" s="39"/>
+      <c r="AB10" s="39"/>
+      <c r="AC10" s="39"/>
+      <c r="AD10" s="39"/>
+      <c r="AE10" s="39"/>
+      <c r="AF10" s="39"/>
       <c r="AG10" s="18" t="s">
         <v>6</v>
       </c>
@@ -1520,37 +1509,37 @@
       <c r="AM10" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="AN10" s="44"/>
-      <c r="AO10" s="52"/>
-      <c r="AP10" s="44"/>
-      <c r="AQ10" s="52"/>
-      <c r="AR10" s="52"/>
-      <c r="AS10" s="44"/>
-      <c r="AT10" s="44"/>
-      <c r="AU10" s="44"/>
-      <c r="AV10" s="44"/>
-      <c r="AW10" s="42"/>
-      <c r="AX10" s="42"/>
-      <c r="AY10" s="42"/>
-      <c r="AZ10" s="42"/>
-      <c r="BA10" s="42"/>
-      <c r="BB10" s="42"/>
-      <c r="BC10" s="42"/>
-      <c r="BD10" s="42"/>
-      <c r="BE10" s="54"/>
-      <c r="BF10" s="42"/>
-      <c r="BG10" s="42"/>
-      <c r="BH10" s="42"/>
-      <c r="BI10" s="42"/>
-      <c r="BJ10" s="42"/>
-      <c r="BK10" s="42"/>
-      <c r="BL10" s="26" t="s">
+      <c r="AN10" s="41"/>
+      <c r="AO10" s="44"/>
+      <c r="AP10" s="41"/>
+      <c r="AQ10" s="44"/>
+      <c r="AR10" s="44"/>
+      <c r="AS10" s="41"/>
+      <c r="AT10" s="41"/>
+      <c r="AU10" s="41"/>
+      <c r="AV10" s="41"/>
+      <c r="AW10" s="39"/>
+      <c r="AX10" s="39"/>
+      <c r="AY10" s="39"/>
+      <c r="AZ10" s="39"/>
+      <c r="BA10" s="39"/>
+      <c r="BB10" s="39"/>
+      <c r="BC10" s="39"/>
+      <c r="BD10" s="39"/>
+      <c r="BE10" s="46"/>
+      <c r="BF10" s="39"/>
+      <c r="BG10" s="39"/>
+      <c r="BH10" s="39"/>
+      <c r="BI10" s="39"/>
+      <c r="BJ10" s="39"/>
+      <c r="BK10" s="39"/>
+      <c r="BL10" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="BM10" s="27" t="s">
+      <c r="BM10" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="BN10" s="42"/>
+      <c r="BN10" s="39"/>
       <c r="BO10" s="12" t="s">
         <v>26</v>
       </c>
@@ -1576,7 +1565,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:75">
+    <row r="11" spans="1:76">
       <c r="A11" s="17" t="s">
         <v>63</v>
       </c>
@@ -1586,10 +1575,10 @@
       <c r="C11" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="29" t="s">
         <v>67</v>
       </c>
       <c r="F11" s="17" t="s">
@@ -1625,26 +1614,26 @@
       <c r="P11" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="Q11" s="35" t="e">
+      <c r="Q11" s="34" t="e">
         <f>R11+S11+T11+U11+V11+W11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R11" s="31" t="s">
+      <c r="R11" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="S11" s="31" t="s">
+      <c r="S11" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="T11" s="31" t="s">
+      <c r="T11" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="U11" s="31" t="s">
+      <c r="U11" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="V11" s="31" t="s">
+      <c r="V11" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="W11" s="31" t="s">
+      <c r="W11" s="30" t="s">
         <v>83</v>
       </c>
       <c r="X11" s="17" t="s">
@@ -1674,26 +1663,26 @@
       <c r="AF11" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="AG11" s="36" t="e">
+      <c r="AG11" s="35" t="e">
         <f>IF((AH11+AI11+AJ11+AK11+AL11+AM11)&gt;0,AH11+AI11+AJ11+AK11+AL11+AM11,)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AH11" s="31" t="s">
+      <c r="AH11" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="AI11" s="31" t="s">
+      <c r="AI11" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AJ11" s="31" t="s">
+      <c r="AJ11" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="AK11" s="31" t="s">
+      <c r="AK11" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="AL11" s="31" t="s">
+      <c r="AL11" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="AM11" s="31" t="s">
+      <c r="AM11" s="30" t="s">
         <v>99</v>
       </c>
       <c r="AN11" s="17" t="s">
@@ -1705,13 +1694,13 @@
       <c r="AP11" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="AQ11" s="32" t="s">
+      <c r="AQ11" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="AR11" s="32" t="s">
+      <c r="AR11" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="AS11" s="32" t="s">
+      <c r="AS11" s="31" t="s">
         <v>130</v>
       </c>
       <c r="AT11" s="17" t="s">
@@ -1732,13 +1721,13 @@
       <c r="AY11" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="AZ11" s="23" t="s">
+      <c r="AZ11" s="22" t="s">
         <v>111</v>
       </c>
       <c r="BA11" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="BB11" s="37" t="e">
+      <c r="BB11" s="36" t="e">
         <f>IF(BJ11&lt;=EOMONTH(AZ11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
@@ -1751,75 +1740,76 @@
       <c r="BE11" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="BF11" s="37" t="e">
+      <c r="BF11" s="36" t="e">
         <f>IF(BJ11&lt;=EOMONTH(AZ11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BG11" s="37" t="e">
+      <c r="BG11" s="36" t="e">
         <f>IF(AND(BJ11&gt;=EOMONTH(AZ11,13),BJ11&lt;=EOMONTH(AZ11,48)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BH11" s="37" t="e">
+      <c r="BH11" s="36" t="e">
         <f>IF(AND(BJ11&gt;=EOMONTH(AZ11,48),BJ11&lt;=EOMONTH(AZ11,72)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BI11" s="37" t="e">
+      <c r="BI11" s="36" t="e">
         <f>IF(BJ11&gt;=EOMONTH(AZ11,73),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BJ11" s="23" t="s">
+      <c r="BJ11" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="BK11" s="23" t="s">
+      <c r="BK11" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="BL11" s="33" t="e">
+      <c r="BL11" s="32" t="e">
         <f>NETWORKDAYS((BJ11-DAY(BJ11)+1),(EOMONTH(BJ11,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BM11" s="33" t="e">
+      <c r="BM11" s="32" t="e">
         <f>NETWORKDAYS(BJ11,BK11)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BN11" s="39" t="e">
+      <c r="BN11" s="38" t="e">
         <f>BM11/BL11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BO11" s="34" t="s">
+      <c r="BO11" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="BP11" s="34" t="s">
+      <c r="BP11" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="BQ11" s="34" t="s">
+      <c r="BQ11" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="BR11" s="24" t="s">
+      <c r="BR11" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="BS11" s="55" t="e">
+      <c r="BS11" s="38" t="e">
         <f>BQ11*BN11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BT11" s="24" t="s">
+      <c r="BT11" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="BU11" s="24" t="s">
+      <c r="BU11" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="BV11" s="25" t="s">
+      <c r="BV11" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="BW11" s="22" t="s">
+      <c r="BW11" s="54" t="s">
         <v>125</v>
       </c>
+      <c r="BX11" s="14"/>
     </row>
-    <row r="12" spans="1:75">
+    <row r="12" spans="1:76">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12"/>
     </row>
-    <row r="13" spans="1:75">
+    <row r="13" spans="1:76">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
@@ -1828,48 +1818,46 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="16" spans="1:75">
+    <row r="16" spans="1:76">
       <c r="AZ16" s="7"/>
       <c r="BJ16" s="7"/>
     </row>
     <row r="18" spans="58:61">
-      <c r="BF18" s="28"/>
+      <c r="BF18" s="27"/>
     </row>
     <row r="22" spans="58:61">
-      <c r="BG22" s="28"/>
-      <c r="BH22" s="28"/>
-      <c r="BI22" s="28"/>
+      <c r="BG22" s="27"/>
+      <c r="BH22" s="27"/>
+      <c r="BI22" s="27"/>
     </row>
     <row r="23" spans="58:61">
-      <c r="BG23" s="28"/>
-      <c r="BH23" s="28"/>
-      <c r="BI23" s="28"/>
+      <c r="BG23" s="27"/>
+      <c r="BH23" s="27"/>
+      <c r="BI23" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="BO9:BS9"/>
-    <mergeCell ref="AN9:AN10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AT9:AT10"/>
-    <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BJ9:BJ10"/>
-    <mergeCell ref="BK9:BK10"/>
-    <mergeCell ref="BN9:BN10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AL9"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:W8"/>
+    <mergeCell ref="X8:AM8"/>
+    <mergeCell ref="AN8:AP8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:V9"/>
+    <mergeCell ref="X9:X10"/>
     <mergeCell ref="AQ8:AU8"/>
     <mergeCell ref="AV8:AV10"/>
     <mergeCell ref="AW8:AW10"/>
@@ -1886,27 +1874,29 @@
     <mergeCell ref="BG9:BG10"/>
     <mergeCell ref="BH9:BH10"/>
     <mergeCell ref="BT9:BV9"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:W8"/>
-    <mergeCell ref="X8:AM8"/>
-    <mergeCell ref="AN8:AP8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:V9"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AL9"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="BO9:BS9"/>
+    <mergeCell ref="AN9:AN10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AU10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BJ9:BJ10"/>
+    <mergeCell ref="BK9:BK10"/>
+    <mergeCell ref="BN9:BN10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
EBEGU-1320: Statistik: Neue Spalte für Betreuungsstatus
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="606"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="135">
   <si>
     <t>Parameter</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t>{eingeschult}</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>{betreuungsStatus}</t>
   </si>
 </sst>
 </file>
@@ -584,7 +590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -656,15 +662,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -680,28 +708,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1068,10 +1077,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BX23"/>
+  <dimension ref="A1:BY23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BF1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BN11" sqref="BN11"/>
+      <selection activeCell="BN9" sqref="BN9:BN10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1102,17 +1111,18 @@
     <col min="62" max="63" width="12.7109375"/>
     <col min="64" max="64" width="11.28515625" hidden="1" customWidth="1"/>
     <col min="65" max="65" width="16" hidden="1" customWidth="1"/>
-    <col min="66" max="67" width="12.7109375"/>
-    <col min="68" max="68" width="16.85546875"/>
-    <col min="69" max="69" width="12.7109375"/>
-    <col min="70" max="70" width="19.42578125"/>
-    <col min="71" max="71" width="16.85546875"/>
-    <col min="72" max="74" width="12.7109375"/>
-    <col min="75" max="75" width="13.42578125" customWidth="1"/>
-    <col min="76" max="1029" width="10.5703125"/>
+    <col min="66" max="66" width="16" customWidth="1"/>
+    <col min="67" max="68" width="12.7109375"/>
+    <col min="69" max="69" width="16.85546875"/>
+    <col min="70" max="70" width="12.7109375"/>
+    <col min="71" max="71" width="19.42578125"/>
+    <col min="72" max="72" width="16.85546875"/>
+    <col min="73" max="75" width="12.7109375"/>
+    <col min="76" max="76" width="13.42578125" customWidth="1"/>
+    <col min="77" max="1030" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" ht="21">
+    <row r="1" spans="1:77" ht="21">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -1123,10 +1133,10 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:76">
+    <row r="2" spans="1:77">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:76">
+    <row r="3" spans="1:77">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1138,8 +1148,9 @@
       <c r="G3" s="4"/>
       <c r="BL3" s="37"/>
       <c r="BM3" s="37"/>
+      <c r="BN3" s="37"/>
     </row>
-    <row r="4" spans="1:76">
+    <row r="4" spans="1:77">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1148,7 +1159,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:76">
+    <row r="5" spans="1:77">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1157,7 +1168,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:76">
+    <row r="6" spans="1:77">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1169,89 +1180,89 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
     </row>
-    <row r="8" spans="1:76" s="13" customFormat="1">
-      <c r="A8" s="50" t="s">
+    <row r="8" spans="1:77" s="13" customFormat="1">
+      <c r="A8" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="50" t="s">
+      <c r="E8" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="50" t="s">
+      <c r="F8" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="50" t="s">
+      <c r="G8" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
-      <c r="T8" s="51"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="51"/>
-      <c r="X8" s="39" t="s">
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="43"/>
+      <c r="W8" s="43"/>
+      <c r="X8" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="Y8" s="39"/>
-      <c r="Z8" s="39"/>
-      <c r="AA8" s="39"/>
-      <c r="AB8" s="39"/>
-      <c r="AC8" s="39"/>
-      <c r="AD8" s="39"/>
-      <c r="AE8" s="39"/>
-      <c r="AF8" s="39"/>
-      <c r="AG8" s="51"/>
-      <c r="AH8" s="51"/>
-      <c r="AI8" s="51"/>
-      <c r="AJ8" s="51"/>
-      <c r="AK8" s="51"/>
-      <c r="AL8" s="51"/>
-      <c r="AM8" s="51"/>
-      <c r="AN8" s="41" t="s">
+      <c r="Y8" s="42"/>
+      <c r="Z8" s="42"/>
+      <c r="AA8" s="42"/>
+      <c r="AB8" s="42"/>
+      <c r="AC8" s="42"/>
+      <c r="AD8" s="42"/>
+      <c r="AE8" s="42"/>
+      <c r="AF8" s="42"/>
+      <c r="AG8" s="43"/>
+      <c r="AH8" s="43"/>
+      <c r="AI8" s="43"/>
+      <c r="AJ8" s="43"/>
+      <c r="AK8" s="43"/>
+      <c r="AL8" s="43"/>
+      <c r="AM8" s="43"/>
+      <c r="AN8" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="AO8" s="41"/>
-      <c r="AP8" s="41"/>
-      <c r="AQ8" s="41" t="s">
+      <c r="AO8" s="44"/>
+      <c r="AP8" s="44"/>
+      <c r="AQ8" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="AR8" s="41"/>
-      <c r="AS8" s="41"/>
-      <c r="AT8" s="41"/>
-      <c r="AU8" s="41"/>
-      <c r="AV8" s="41" t="s">
+      <c r="AR8" s="44"/>
+      <c r="AS8" s="44"/>
+      <c r="AT8" s="44"/>
+      <c r="AU8" s="44"/>
+      <c r="AV8" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="AW8" s="39" t="s">
+      <c r="AW8" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="AX8" s="39" t="s">
+      <c r="AX8" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="AY8" s="39"/>
-      <c r="AZ8" s="39"/>
-      <c r="BA8" s="39"/>
-      <c r="BB8" s="39"/>
+      <c r="AY8" s="42"/>
+      <c r="AZ8" s="42"/>
+      <c r="BA8" s="42"/>
+      <c r="BB8" s="42"/>
       <c r="BC8" s="11"/>
       <c r="BD8" s="11"/>
       <c r="BE8" s="28"/>
@@ -1259,205 +1270,209 @@
       <c r="BG8" s="11"/>
       <c r="BH8" s="11"/>
       <c r="BI8" s="11"/>
-      <c r="BJ8" s="39" t="s">
+      <c r="BJ8" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="BK8" s="39"/>
-      <c r="BL8" s="39"/>
-      <c r="BM8" s="39"/>
-      <c r="BN8" s="39"/>
-      <c r="BO8" s="39"/>
-      <c r="BP8" s="39"/>
-      <c r="BQ8" s="39"/>
-      <c r="BR8" s="39"/>
-      <c r="BS8" s="39"/>
-      <c r="BT8" s="39"/>
-      <c r="BU8" s="39"/>
-      <c r="BV8" s="39"/>
+      <c r="BK8" s="42"/>
+      <c r="BL8" s="42"/>
+      <c r="BM8" s="42"/>
+      <c r="BN8" s="42"/>
+      <c r="BO8" s="42"/>
+      <c r="BP8" s="42"/>
+      <c r="BQ8" s="42"/>
+      <c r="BR8" s="42"/>
+      <c r="BS8" s="42"/>
+      <c r="BT8" s="42"/>
+      <c r="BU8" s="42"/>
+      <c r="BV8" s="42"/>
+      <c r="BW8" s="42"/>
     </row>
-    <row r="9" spans="1:76">
-      <c r="A9" s="50"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="39" t="s">
+    <row r="9" spans="1:77">
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="39" t="s">
+      <c r="I9" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="K9" s="39" t="s">
+      <c r="K9" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="L9" s="39" t="s">
+      <c r="L9" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="M9" s="39" t="s">
+      <c r="M9" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="N9" s="39" t="s">
+      <c r="N9" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="47" t="s">
+      <c r="P9" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="Q9" s="47" t="s">
+      <c r="Q9" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="R9" s="48"/>
-      <c r="S9" s="48"/>
-      <c r="T9" s="48"/>
-      <c r="U9" s="48"/>
-      <c r="V9" s="48"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="46"/>
+      <c r="V9" s="46"/>
       <c r="W9" s="15"/>
-      <c r="X9" s="52" t="s">
+      <c r="X9" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="Y9" s="39" t="s">
+      <c r="Y9" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="Z9" s="39" t="s">
+      <c r="Z9" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="AA9" s="39" t="s">
+      <c r="AA9" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="AB9" s="39" t="s">
+      <c r="AB9" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="AC9" s="39" t="s">
+      <c r="AC9" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="AD9" s="39" t="s">
+      <c r="AD9" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="AE9" s="39" t="s">
+      <c r="AE9" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="AF9" s="47" t="s">
+      <c r="AF9" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="AG9" s="47" t="s">
+      <c r="AG9" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="AH9" s="48"/>
-      <c r="AI9" s="48"/>
-      <c r="AJ9" s="48"/>
-      <c r="AK9" s="48"/>
-      <c r="AL9" s="48"/>
+      <c r="AH9" s="46"/>
+      <c r="AI9" s="46"/>
+      <c r="AJ9" s="46"/>
+      <c r="AK9" s="46"/>
+      <c r="AL9" s="46"/>
       <c r="AM9" s="15"/>
-      <c r="AN9" s="40" t="s">
+      <c r="AN9" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="AO9" s="43" t="s">
+      <c r="AO9" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="AP9" s="41" t="s">
+      <c r="AP9" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="AQ9" s="43" t="s">
+      <c r="AQ9" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="AR9" s="43" t="s">
+      <c r="AR9" s="51" t="s">
         <v>128</v>
       </c>
-      <c r="AS9" s="41" t="s">
+      <c r="AS9" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="AT9" s="42" t="s">
+      <c r="AT9" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="AU9" s="41" t="s">
+      <c r="AU9" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="AV9" s="41"/>
-      <c r="AW9" s="39"/>
-      <c r="AX9" s="39" t="s">
+      <c r="AV9" s="44"/>
+      <c r="AW9" s="42"/>
+      <c r="AX9" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="AY9" s="39" t="s">
+      <c r="AY9" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="AZ9" s="39" t="s">
+      <c r="AZ9" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="BA9" s="49" t="s">
+      <c r="BA9" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="BB9" s="39" t="s">
+      <c r="BB9" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="BC9" s="39" t="s">
+      <c r="BC9" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="BD9" s="39" t="s">
+      <c r="BD9" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="BE9" s="45" t="s">
+      <c r="BE9" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="BF9" s="39" t="s">
+      <c r="BF9" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BG9" s="39" t="s">
+      <c r="BG9" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="BH9" s="39" t="s">
+      <c r="BH9" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="BI9" s="39" t="s">
+      <c r="BI9" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="BJ9" s="39" t="s">
+      <c r="BJ9" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="BK9" s="39" t="s">
+      <c r="BK9" s="42" t="s">
         <v>5</v>
       </c>
       <c r="BL9" s="25"/>
       <c r="BM9" s="25"/>
-      <c r="BN9" s="39" t="s">
+      <c r="BN9" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="BO9" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="BO9" s="39" t="s">
+      <c r="BP9" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="BP9" s="39"/>
-      <c r="BQ9" s="39"/>
-      <c r="BR9" s="39"/>
-      <c r="BS9" s="39"/>
-      <c r="BT9" s="39" t="s">
+      <c r="BQ9" s="42"/>
+      <c r="BR9" s="42"/>
+      <c r="BS9" s="42"/>
+      <c r="BT9" s="42"/>
+      <c r="BU9" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="BU9" s="39"/>
-      <c r="BV9" s="39"/>
+      <c r="BV9" s="42"/>
+      <c r="BW9" s="42"/>
     </row>
-    <row r="10" spans="1:76">
-      <c r="A10" s="50"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
+    <row r="10" spans="1:77">
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="42"/>
       <c r="Q10" s="18" t="s">
         <v>6</v>
       </c>
@@ -1479,15 +1494,15 @@
       <c r="W10" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="X10" s="39"/>
-      <c r="Y10" s="39"/>
-      <c r="Z10" s="39"/>
-      <c r="AA10" s="39"/>
-      <c r="AB10" s="39"/>
-      <c r="AC10" s="39"/>
-      <c r="AD10" s="39"/>
-      <c r="AE10" s="39"/>
-      <c r="AF10" s="39"/>
+      <c r="X10" s="42"/>
+      <c r="Y10" s="42"/>
+      <c r="Z10" s="42"/>
+      <c r="AA10" s="42"/>
+      <c r="AB10" s="42"/>
+      <c r="AC10" s="42"/>
+      <c r="AD10" s="42"/>
+      <c r="AE10" s="42"/>
+      <c r="AF10" s="42"/>
       <c r="AG10" s="18" t="s">
         <v>6</v>
       </c>
@@ -1509,63 +1524,64 @@
       <c r="AM10" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="AN10" s="41"/>
-      <c r="AO10" s="44"/>
-      <c r="AP10" s="41"/>
-      <c r="AQ10" s="44"/>
-      <c r="AR10" s="44"/>
-      <c r="AS10" s="41"/>
-      <c r="AT10" s="41"/>
-      <c r="AU10" s="41"/>
-      <c r="AV10" s="41"/>
-      <c r="AW10" s="39"/>
-      <c r="AX10" s="39"/>
-      <c r="AY10" s="39"/>
-      <c r="AZ10" s="39"/>
-      <c r="BA10" s="39"/>
-      <c r="BB10" s="39"/>
-      <c r="BC10" s="39"/>
-      <c r="BD10" s="39"/>
-      <c r="BE10" s="46"/>
-      <c r="BF10" s="39"/>
-      <c r="BG10" s="39"/>
-      <c r="BH10" s="39"/>
-      <c r="BI10" s="39"/>
-      <c r="BJ10" s="39"/>
-      <c r="BK10" s="39"/>
+      <c r="AN10" s="44"/>
+      <c r="AO10" s="52"/>
+      <c r="AP10" s="44"/>
+      <c r="AQ10" s="52"/>
+      <c r="AR10" s="52"/>
+      <c r="AS10" s="44"/>
+      <c r="AT10" s="44"/>
+      <c r="AU10" s="44"/>
+      <c r="AV10" s="44"/>
+      <c r="AW10" s="42"/>
+      <c r="AX10" s="42"/>
+      <c r="AY10" s="42"/>
+      <c r="AZ10" s="42"/>
+      <c r="BA10" s="42"/>
+      <c r="BB10" s="42"/>
+      <c r="BC10" s="42"/>
+      <c r="BD10" s="42"/>
+      <c r="BE10" s="54"/>
+      <c r="BF10" s="42"/>
+      <c r="BG10" s="42"/>
+      <c r="BH10" s="42"/>
+      <c r="BI10" s="42"/>
+      <c r="BJ10" s="42"/>
+      <c r="BK10" s="42"/>
       <c r="BL10" s="25" t="s">
         <v>56</v>
       </c>
       <c r="BM10" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="BN10" s="39"/>
-      <c r="BO10" s="12" t="s">
+      <c r="BN10" s="55"/>
+      <c r="BO10" s="42"/>
+      <c r="BP10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="BP10" s="12" t="s">
+      <c r="BQ10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="BQ10" s="12" t="s">
+      <c r="BR10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="BR10" s="12" t="s">
+      <c r="BS10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="BS10" s="12" t="s">
+      <c r="BT10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="BT10" s="12" t="s">
+      <c r="BU10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="BU10" s="12" t="s">
+      <c r="BV10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="BV10" s="12" t="s">
+      <c r="BW10" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:76">
+    <row r="11" spans="1:77">
       <c r="A11" s="17" t="s">
         <v>63</v>
       </c>
@@ -1770,46 +1786,49 @@
         <f>NETWORKDAYS(BJ11,BK11)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BN11" s="38" t="e">
+      <c r="BN11" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="BO11" s="38" t="e">
         <f>BM11/BL11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BO11" s="33" t="s">
+      <c r="BP11" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="BP11" s="33" t="s">
+      <c r="BQ11" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="BQ11" s="33" t="s">
+      <c r="BR11" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="BR11" s="23" t="s">
+      <c r="BS11" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="BS11" s="38" t="e">
-        <f>BQ11*BN11</f>
+      <c r="BT11" s="38" t="e">
+        <f>BR11*BO11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BT11" s="23" t="s">
+      <c r="BU11" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="BU11" s="23" t="s">
+      <c r="BV11" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="BV11" s="24" t="s">
+      <c r="BW11" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="BW11" s="54" t="s">
+      <c r="BX11" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="BX11" s="14"/>
+      <c r="BY11" s="14"/>
     </row>
-    <row r="12" spans="1:76">
+    <row r="12" spans="1:77">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12"/>
     </row>
-    <row r="13" spans="1:76">
+    <row r="13" spans="1:77">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
@@ -1818,7 +1837,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="16" spans="1:76">
+    <row r="16" spans="1:77">
       <c r="AZ16" s="7"/>
       <c r="BJ16" s="7"/>
     </row>
@@ -1836,12 +1855,47 @@
       <c r="BI23" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
+  <mergeCells count="61">
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="AN9:AN10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AU10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BJ9:BJ10"/>
+    <mergeCell ref="BK9:BK10"/>
+    <mergeCell ref="BO9:BO10"/>
+    <mergeCell ref="BN9:BN10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AL9"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AQ8:AU8"/>
+    <mergeCell ref="AV8:AV10"/>
+    <mergeCell ref="AW8:AW10"/>
+    <mergeCell ref="AX8:BB8"/>
+    <mergeCell ref="BJ8:BW8"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="AZ9:AZ10"/>
+    <mergeCell ref="BA9:BA10"/>
+    <mergeCell ref="BB9:BB10"/>
+    <mergeCell ref="BC9:BC10"/>
+    <mergeCell ref="BD9:BD10"/>
+    <mergeCell ref="BF9:BF10"/>
+    <mergeCell ref="BG9:BG10"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="BU9:BW9"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="G8:G10"/>
     <mergeCell ref="H8:W8"/>
@@ -1858,45 +1912,11 @@
     <mergeCell ref="P9:P10"/>
     <mergeCell ref="Q9:V9"/>
     <mergeCell ref="X9:X10"/>
-    <mergeCell ref="AQ8:AU8"/>
-    <mergeCell ref="AV8:AV10"/>
-    <mergeCell ref="AW8:AW10"/>
-    <mergeCell ref="AX8:BB8"/>
-    <mergeCell ref="BJ8:BV8"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="AZ9:AZ10"/>
-    <mergeCell ref="BA9:BA10"/>
-    <mergeCell ref="BB9:BB10"/>
-    <mergeCell ref="BC9:BC10"/>
-    <mergeCell ref="BD9:BD10"/>
-    <mergeCell ref="BF9:BF10"/>
-    <mergeCell ref="BG9:BG10"/>
-    <mergeCell ref="BH9:BH10"/>
-    <mergeCell ref="BT9:BV9"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AL9"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="BO9:BS9"/>
-    <mergeCell ref="AN9:AN10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AT9:AT10"/>
-    <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BJ9:BJ10"/>
-    <mergeCell ref="BK9:BK10"/>
-    <mergeCell ref="BN9:BN10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
EBEGU-1552 * Report rows now exported via ExcelMerger RollFiller * Excel Merger 2.0.5-SNAPSHOT is awaiting review and release build
EBEGU-1545
* ReportService fetches latest Gesuch via GesuchService if not latest valid Gesuch
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchstellerKinderBetreuung.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11129"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/medu/dev/ebegu/ebegu-server/src/main/resources/reporting/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="606"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20560" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -429,11 +434,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -590,7 +595,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -604,7 +609,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -648,7 +652,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -662,59 +665,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -786,13 +789,21 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -830,9 +841,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -864,9 +875,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -898,9 +927,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1073,56 +1120,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BY23"/>
+  <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BF1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BN9" sqref="BN9:BN10"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BP17" sqref="BP17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.7109375"/>
-    <col min="3" max="3" width="15.7109375" style="1"/>
+    <col min="1" max="2" width="20.6640625"/>
+    <col min="3" max="3" width="15.6640625" style="1"/>
     <col min="4" max="5" width="17"/>
-    <col min="8" max="16" width="8.7109375"/>
-    <col min="17" max="22" width="10.7109375"/>
-    <col min="23" max="23" width="24.140625"/>
-    <col min="24" max="32" width="8.7109375"/>
-    <col min="33" max="38" width="10.7109375"/>
-    <col min="39" max="39" width="24.140625"/>
-    <col min="40" max="40" width="9.140625" customWidth="1"/>
-    <col min="42" max="42" width="6.5703125"/>
-    <col min="43" max="43" width="18.140625"/>
-    <col min="45" max="45" width="23.28515625"/>
-    <col min="46" max="46" width="9.28515625"/>
-    <col min="47" max="47" width="25.42578125"/>
-    <col min="48" max="48" width="27.5703125"/>
-    <col min="49" max="49" width="10.5703125"/>
-    <col min="50" max="52" width="12.7109375"/>
-    <col min="53" max="53" width="16.7109375"/>
-    <col min="54" max="55" width="12.7109375"/>
+    <col min="8" max="16" width="8.6640625"/>
+    <col min="17" max="22" width="10.6640625"/>
+    <col min="23" max="23" width="24.1640625"/>
+    <col min="24" max="32" width="8.6640625"/>
+    <col min="33" max="38" width="10.6640625"/>
+    <col min="39" max="39" width="24.1640625"/>
+    <col min="40" max="40" width="9.1640625" customWidth="1"/>
+    <col min="42" max="42" width="6.5"/>
+    <col min="43" max="43" width="18.1640625"/>
+    <col min="45" max="45" width="23.33203125"/>
+    <col min="46" max="46" width="9.33203125"/>
+    <col min="47" max="47" width="25.5"/>
+    <col min="48" max="48" width="27.5"/>
+    <col min="49" max="49" width="10.5"/>
+    <col min="50" max="52" width="12.6640625"/>
+    <col min="53" max="53" width="16.6640625"/>
+    <col min="54" max="55" width="12.6640625"/>
     <col min="56" max="56" width="22"/>
-    <col min="57" max="57" width="10.85546875" customWidth="1"/>
+    <col min="57" max="57" width="10.83203125" customWidth="1"/>
     <col min="58" max="61" width="22"/>
-    <col min="62" max="63" width="12.7109375"/>
-    <col min="64" max="64" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="62" max="63" width="12.6640625"/>
+    <col min="64" max="64" width="11.33203125" hidden="1" customWidth="1"/>
     <col min="65" max="65" width="16" hidden="1" customWidth="1"/>
     <col min="66" max="66" width="16" customWidth="1"/>
-    <col min="67" max="68" width="12.7109375"/>
-    <col min="69" max="69" width="16.85546875"/>
-    <col min="70" max="70" width="12.7109375"/>
-    <col min="71" max="71" width="19.42578125"/>
-    <col min="72" max="72" width="16.85546875"/>
-    <col min="73" max="75" width="12.7109375"/>
-    <col min="76" max="76" width="13.42578125" customWidth="1"/>
-    <col min="77" max="1030" width="10.5703125"/>
+    <col min="67" max="68" width="12.6640625"/>
+    <col min="69" max="69" width="16.83203125"/>
+    <col min="70" max="70" width="12.6640625"/>
+    <col min="71" max="71" width="19.5"/>
+    <col min="72" max="72" width="16.83203125"/>
+    <col min="73" max="75" width="12.6640625"/>
+    <col min="76" max="996" width="10.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="21">
+    <row r="1" spans="1:77" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -1133,10 +1179,10 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:77">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.2">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:77">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1146,11 +1192,11 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="BL3" s="37"/>
-      <c r="BM3" s="37"/>
-      <c r="BN3" s="37"/>
+      <c r="BL3" s="35"/>
+      <c r="BM3" s="35"/>
+      <c r="BN3" s="35"/>
     </row>
-    <row r="4" spans="1:77">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1159,7 +1205,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:77">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1168,718 +1214,687 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:77">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
     </row>
-    <row r="8" spans="1:77" s="13" customFormat="1">
-      <c r="A8" s="40" t="s">
+    <row r="7" spans="1:77" x14ac:dyDescent="0.2">
+      <c r="C7"/>
+    </row>
+    <row r="8" spans="1:77" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="40" t="s">
+      <c r="G8" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="42" t="s">
+      <c r="H8" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="43"/>
-      <c r="S8" s="43"/>
-      <c r="T8" s="43"/>
-      <c r="U8" s="43"/>
-      <c r="V8" s="43"/>
-      <c r="W8" s="43"/>
-      <c r="X8" s="42" t="s">
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="50"/>
+      <c r="S8" s="50"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="50"/>
+      <c r="V8" s="50"/>
+      <c r="W8" s="50"/>
+      <c r="X8" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="Y8" s="42"/>
-      <c r="Z8" s="42"/>
-      <c r="AA8" s="42"/>
-      <c r="AB8" s="42"/>
-      <c r="AC8" s="42"/>
-      <c r="AD8" s="42"/>
-      <c r="AE8" s="42"/>
-      <c r="AF8" s="42"/>
-      <c r="AG8" s="43"/>
-      <c r="AH8" s="43"/>
-      <c r="AI8" s="43"/>
-      <c r="AJ8" s="43"/>
-      <c r="AK8" s="43"/>
-      <c r="AL8" s="43"/>
-      <c r="AM8" s="43"/>
-      <c r="AN8" s="44" t="s">
+      <c r="Y8" s="37"/>
+      <c r="Z8" s="37"/>
+      <c r="AA8" s="37"/>
+      <c r="AB8" s="37"/>
+      <c r="AC8" s="37"/>
+      <c r="AD8" s="37"/>
+      <c r="AE8" s="37"/>
+      <c r="AF8" s="37"/>
+      <c r="AG8" s="50"/>
+      <c r="AH8" s="50"/>
+      <c r="AI8" s="50"/>
+      <c r="AJ8" s="50"/>
+      <c r="AK8" s="50"/>
+      <c r="AL8" s="50"/>
+      <c r="AM8" s="50"/>
+      <c r="AN8" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="AO8" s="44"/>
-      <c r="AP8" s="44"/>
-      <c r="AQ8" s="44" t="s">
+      <c r="AO8" s="39"/>
+      <c r="AP8" s="39"/>
+      <c r="AQ8" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="AR8" s="44"/>
-      <c r="AS8" s="44"/>
-      <c r="AT8" s="44"/>
-      <c r="AU8" s="44"/>
-      <c r="AV8" s="44" t="s">
+      <c r="AR8" s="39"/>
+      <c r="AS8" s="39"/>
+      <c r="AT8" s="39"/>
+      <c r="AU8" s="39"/>
+      <c r="AV8" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="AW8" s="42" t="s">
+      <c r="AW8" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="AX8" s="42" t="s">
+      <c r="AX8" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="AY8" s="42"/>
-      <c r="AZ8" s="42"/>
-      <c r="BA8" s="42"/>
-      <c r="BB8" s="42"/>
-      <c r="BC8" s="11"/>
-      <c r="BD8" s="11"/>
-      <c r="BE8" s="28"/>
-      <c r="BF8" s="11"/>
-      <c r="BG8" s="11"/>
-      <c r="BH8" s="11"/>
-      <c r="BI8" s="11"/>
-      <c r="BJ8" s="42" t="s">
+      <c r="AY8" s="37"/>
+      <c r="AZ8" s="37"/>
+      <c r="BA8" s="37"/>
+      <c r="BB8" s="37"/>
+      <c r="BC8" s="10"/>
+      <c r="BD8" s="10"/>
+      <c r="BE8" s="26"/>
+      <c r="BF8" s="10"/>
+      <c r="BG8" s="10"/>
+      <c r="BH8" s="10"/>
+      <c r="BI8" s="10"/>
+      <c r="BJ8" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="BK8" s="42"/>
-      <c r="BL8" s="42"/>
-      <c r="BM8" s="42"/>
-      <c r="BN8" s="42"/>
-      <c r="BO8" s="42"/>
-      <c r="BP8" s="42"/>
-      <c r="BQ8" s="42"/>
-      <c r="BR8" s="42"/>
-      <c r="BS8" s="42"/>
-      <c r="BT8" s="42"/>
-      <c r="BU8" s="42"/>
-      <c r="BV8" s="42"/>
-      <c r="BW8" s="42"/>
+      <c r="BK8" s="37"/>
+      <c r="BL8" s="37"/>
+      <c r="BM8" s="37"/>
+      <c r="BN8" s="37"/>
+      <c r="BO8" s="37"/>
+      <c r="BP8" s="37"/>
+      <c r="BQ8" s="37"/>
+      <c r="BR8" s="37"/>
+      <c r="BS8" s="37"/>
+      <c r="BT8" s="37"/>
+      <c r="BU8" s="37"/>
+      <c r="BV8" s="37"/>
+      <c r="BW8" s="37"/>
     </row>
-    <row r="9" spans="1:77">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="42" t="s">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.2">
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="42" t="s">
+      <c r="J9" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="K9" s="42" t="s">
+      <c r="K9" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="L9" s="42" t="s">
+      <c r="L9" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="M9" s="42" t="s">
+      <c r="M9" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="N9" s="42" t="s">
+      <c r="N9" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="42" t="s">
+      <c r="O9" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="45" t="s">
+      <c r="P9" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="Q9" s="45" t="s">
+      <c r="Q9" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="R9" s="46"/>
-      <c r="S9" s="46"/>
-      <c r="T9" s="46"/>
-      <c r="U9" s="46"/>
-      <c r="V9" s="46"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="47" t="s">
+      <c r="R9" s="47"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="47"/>
+      <c r="V9" s="47"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="Y9" s="42" t="s">
+      <c r="Y9" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="Z9" s="42" t="s">
+      <c r="Z9" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="AA9" s="42" t="s">
+      <c r="AA9" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="AB9" s="42" t="s">
+      <c r="AB9" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="AC9" s="42" t="s">
+      <c r="AC9" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="AD9" s="42" t="s">
+      <c r="AD9" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="AE9" s="42" t="s">
+      <c r="AE9" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="AF9" s="45" t="s">
+      <c r="AF9" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="AG9" s="45" t="s">
+      <c r="AG9" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="AH9" s="46"/>
-      <c r="AI9" s="46"/>
-      <c r="AJ9" s="46"/>
-      <c r="AK9" s="46"/>
-      <c r="AL9" s="46"/>
-      <c r="AM9" s="15"/>
-      <c r="AN9" s="49" t="s">
+      <c r="AH9" s="47"/>
+      <c r="AI9" s="47"/>
+      <c r="AJ9" s="47"/>
+      <c r="AK9" s="47"/>
+      <c r="AL9" s="47"/>
+      <c r="AM9" s="14"/>
+      <c r="AN9" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="AO9" s="51" t="s">
+      <c r="AO9" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="AP9" s="44" t="s">
+      <c r="AP9" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="AQ9" s="51" t="s">
+      <c r="AQ9" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="AR9" s="51" t="s">
+      <c r="AR9" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="AS9" s="44" t="s">
+      <c r="AS9" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="AT9" s="50" t="s">
+      <c r="AT9" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="AU9" s="44" t="s">
+      <c r="AU9" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="AV9" s="44"/>
-      <c r="AW9" s="42"/>
-      <c r="AX9" s="42" t="s">
+      <c r="AV9" s="39"/>
+      <c r="AW9" s="37"/>
+      <c r="AX9" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="AY9" s="42" t="s">
+      <c r="AY9" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="AZ9" s="42" t="s">
+      <c r="AZ9" s="37" t="s">
         <v>18</v>
       </c>
       <c r="BA9" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="BB9" s="42" t="s">
+      <c r="BB9" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="BC9" s="42" t="s">
+      <c r="BC9" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="BD9" s="42" t="s">
+      <c r="BD9" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="BE9" s="53" t="s">
+      <c r="BE9" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="BF9" s="42" t="s">
+      <c r="BF9" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="BG9" s="42" t="s">
+      <c r="BG9" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="BH9" s="42" t="s">
+      <c r="BH9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="BI9" s="42" t="s">
+      <c r="BI9" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="BJ9" s="42" t="s">
+      <c r="BJ9" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="BK9" s="42" t="s">
+      <c r="BK9" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="BL9" s="25"/>
-      <c r="BM9" s="25"/>
-      <c r="BN9" s="53" t="s">
+      <c r="BL9" s="24"/>
+      <c r="BM9" s="24"/>
+      <c r="BN9" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="BO9" s="42" t="s">
+      <c r="BO9" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="BP9" s="42" t="s">
+      <c r="BP9" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="BQ9" s="42"/>
-      <c r="BR9" s="42"/>
-      <c r="BS9" s="42"/>
-      <c r="BT9" s="42"/>
-      <c r="BU9" s="42" t="s">
+      <c r="BQ9" s="37"/>
+      <c r="BR9" s="37"/>
+      <c r="BS9" s="37"/>
+      <c r="BT9" s="37"/>
+      <c r="BU9" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="BV9" s="42"/>
-      <c r="BW9" s="42"/>
+      <c r="BV9" s="37"/>
+      <c r="BW9" s="37"/>
     </row>
-    <row r="10" spans="1:77">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="18" t="s">
+    <row r="10" spans="1:77" x14ac:dyDescent="0.2">
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="R10" s="18" t="s">
+      <c r="R10" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="S10" s="18" t="s">
+      <c r="S10" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="T10" s="18" t="s">
+      <c r="T10" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="U10" s="18" t="s">
+      <c r="U10" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="V10" s="18" t="s">
+      <c r="V10" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="W10" s="19" t="s">
+      <c r="W10" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="X10" s="42"/>
-      <c r="Y10" s="42"/>
-      <c r="Z10" s="42"/>
-      <c r="AA10" s="42"/>
-      <c r="AB10" s="42"/>
-      <c r="AC10" s="42"/>
-      <c r="AD10" s="42"/>
-      <c r="AE10" s="42"/>
-      <c r="AF10" s="42"/>
-      <c r="AG10" s="18" t="s">
+      <c r="X10" s="37"/>
+      <c r="Y10" s="37"/>
+      <c r="Z10" s="37"/>
+      <c r="AA10" s="37"/>
+      <c r="AB10" s="37"/>
+      <c r="AC10" s="37"/>
+      <c r="AD10" s="37"/>
+      <c r="AE10" s="37"/>
+      <c r="AF10" s="37"/>
+      <c r="AG10" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="AH10" s="18" t="s">
+      <c r="AH10" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="AI10" s="18" t="s">
+      <c r="AI10" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AJ10" s="18" t="s">
+      <c r="AJ10" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="AK10" s="18" t="s">
+      <c r="AK10" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="AL10" s="18" t="s">
+      <c r="AL10" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="AM10" s="20" t="s">
+      <c r="AM10" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="AN10" s="44"/>
-      <c r="AO10" s="52"/>
-      <c r="AP10" s="44"/>
-      <c r="AQ10" s="52"/>
-      <c r="AR10" s="52"/>
-      <c r="AS10" s="44"/>
-      <c r="AT10" s="44"/>
-      <c r="AU10" s="44"/>
-      <c r="AV10" s="44"/>
-      <c r="AW10" s="42"/>
-      <c r="AX10" s="42"/>
-      <c r="AY10" s="42"/>
-      <c r="AZ10" s="42"/>
-      <c r="BA10" s="42"/>
-      <c r="BB10" s="42"/>
-      <c r="BC10" s="42"/>
-      <c r="BD10" s="42"/>
-      <c r="BE10" s="54"/>
-      <c r="BF10" s="42"/>
-      <c r="BG10" s="42"/>
-      <c r="BH10" s="42"/>
-      <c r="BI10" s="42"/>
-      <c r="BJ10" s="42"/>
-      <c r="BK10" s="42"/>
-      <c r="BL10" s="25" t="s">
+      <c r="AN10" s="39"/>
+      <c r="AO10" s="42"/>
+      <c r="AP10" s="39"/>
+      <c r="AQ10" s="42"/>
+      <c r="AR10" s="42"/>
+      <c r="AS10" s="39"/>
+      <c r="AT10" s="39"/>
+      <c r="AU10" s="39"/>
+      <c r="AV10" s="39"/>
+      <c r="AW10" s="37"/>
+      <c r="AX10" s="37"/>
+      <c r="AY10" s="37"/>
+      <c r="AZ10" s="37"/>
+      <c r="BA10" s="37"/>
+      <c r="BB10" s="37"/>
+      <c r="BC10" s="37"/>
+      <c r="BD10" s="37"/>
+      <c r="BE10" s="44"/>
+      <c r="BF10" s="37"/>
+      <c r="BG10" s="37"/>
+      <c r="BH10" s="37"/>
+      <c r="BI10" s="37"/>
+      <c r="BJ10" s="37"/>
+      <c r="BK10" s="37"/>
+      <c r="BL10" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="BM10" s="26" t="s">
+      <c r="BM10" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="BN10" s="55"/>
-      <c r="BO10" s="42"/>
-      <c r="BP10" s="12" t="s">
+      <c r="BN10" s="45"/>
+      <c r="BO10" s="37"/>
+      <c r="BP10" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="BQ10" s="12" t="s">
+      <c r="BQ10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="BR10" s="12" t="s">
+      <c r="BR10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="BS10" s="12" t="s">
+      <c r="BS10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="BT10" s="12" t="s">
+      <c r="BT10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="BU10" s="12" t="s">
+      <c r="BU10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="BV10" s="12" t="s">
+      <c r="BV10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="BW10" s="12" t="s">
+      <c r="BW10" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:77">
-      <c r="A11" s="17" t="s">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="L11" s="17" t="s">
+      <c r="L11" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="M11" s="17" t="s">
+      <c r="M11" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="N11" s="17" t="s">
+      <c r="N11" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="O11" s="17" t="s">
+      <c r="O11" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="P11" s="17" t="s">
+      <c r="P11" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="Q11" s="34" t="e">
+      <c r="Q11" s="32" t="e">
         <f>R11+S11+T11+U11+V11+W11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R11" s="30" t="s">
+      <c r="R11" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="S11" s="30" t="s">
+      <c r="S11" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="T11" s="30" t="s">
+      <c r="T11" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="U11" s="30" t="s">
+      <c r="U11" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="V11" s="30" t="s">
+      <c r="V11" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="W11" s="30" t="s">
+      <c r="W11" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="X11" s="17" t="s">
+      <c r="X11" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="Y11" s="17" t="s">
+      <c r="Y11" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Z11" s="17" t="s">
+      <c r="Z11" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="AA11" s="17" t="s">
+      <c r="AA11" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="AB11" s="17" t="s">
+      <c r="AB11" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="AC11" s="17" t="s">
+      <c r="AC11" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="AD11" s="17" t="s">
+      <c r="AD11" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="AE11" s="17" t="s">
+      <c r="AE11" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="AF11" s="17" t="s">
+      <c r="AF11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="AG11" s="35" t="e">
+      <c r="AG11" s="33" t="e">
         <f>IF((AH11+AI11+AJ11+AK11+AL11+AM11)&gt;0,AH11+AI11+AJ11+AK11+AL11+AM11,)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AH11" s="30" t="s">
+      <c r="AH11" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="AI11" s="30" t="s">
+      <c r="AI11" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="AJ11" s="30" t="s">
+      <c r="AJ11" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="AK11" s="30" t="s">
+      <c r="AK11" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="AL11" s="30" t="s">
+      <c r="AL11" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="AM11" s="30" t="s">
+      <c r="AM11" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="AN11" s="17" t="s">
+      <c r="AN11" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="AO11" s="17" t="s">
+      <c r="AO11" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="AP11" s="17" t="s">
+      <c r="AP11" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="AQ11" s="31" t="s">
+      <c r="AQ11" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="AR11" s="31" t="s">
+      <c r="AR11" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="AS11" s="31" t="s">
+      <c r="AS11" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="AT11" s="17" t="s">
+      <c r="AT11" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="AU11" s="17" t="s">
+      <c r="AU11" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="AV11" s="17" t="s">
+      <c r="AV11" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="AW11" s="17" t="s">
+      <c r="AW11" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="AX11" s="21" t="s">
+      <c r="AX11" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="AY11" s="21" t="s">
+      <c r="AY11" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="AZ11" s="22" t="s">
+      <c r="AZ11" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="BA11" s="21" t="s">
+      <c r="BA11" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="BB11" s="36" t="e">
+      <c r="BB11" s="34" t="e">
         <f>IF(BJ11&lt;=EOMONTH(AZ11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BC11" s="21" t="s">
+      <c r="BC11" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="BD11" s="21" t="s">
+      <c r="BD11" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="BE11" s="21" t="s">
+      <c r="BE11" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="BF11" s="36" t="e">
+      <c r="BF11" s="34" t="e">
         <f>IF(BJ11&lt;=EOMONTH(AZ11,12),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BG11" s="36" t="e">
+      <c r="BG11" s="34" t="e">
         <f>IF(AND(BJ11&gt;=EOMONTH(AZ11,13),BJ11&lt;=EOMONTH(AZ11,48)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BH11" s="36" t="e">
+      <c r="BH11" s="34" t="e">
         <f>IF(AND(BJ11&gt;=EOMONTH(AZ11,48),BJ11&lt;=EOMONTH(AZ11,72)),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BI11" s="36" t="e">
+      <c r="BI11" s="34" t="e">
         <f>IF(BJ11&gt;=EOMONTH(AZ11,73),"X","")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BJ11" s="22" t="s">
+      <c r="BJ11" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="BK11" s="22" t="s">
+      <c r="BK11" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="BL11" s="32" t="e">
+      <c r="BL11" s="30" t="e">
         <f>NETWORKDAYS((BJ11-DAY(BJ11)+1),(EOMONTH(BJ11,0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BM11" s="32" t="e">
+      <c r="BM11" s="30" t="e">
         <f>NETWORKDAYS(BJ11,BK11)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BN11" s="32" t="s">
+      <c r="BN11" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="BO11" s="38" t="e">
+      <c r="BO11" s="36" t="e">
         <f>BM11/BL11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BP11" s="33" t="s">
+      <c r="BP11" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="BQ11" s="33" t="s">
+      <c r="BQ11" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="BR11" s="33" t="s">
+      <c r="BR11" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="BS11" s="23" t="s">
+      <c r="BS11" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="BT11" s="38" t="e">
+      <c r="BT11" s="36" t="e">
         <f>BR11*BO11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BU11" s="23" t="s">
+      <c r="BU11" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="BV11" s="23" t="s">
+      <c r="BV11" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="BW11" s="24" t="s">
+      <c r="BW11" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="BX11" s="39" t="s">
+      <c r="BX11" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="BY11" s="14"/>
-    </row>
-    <row r="12" spans="1:77">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12"/>
-    </row>
-    <row r="13" spans="1:77">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="16" spans="1:77">
-      <c r="AZ16" s="7"/>
-      <c r="BJ16" s="7"/>
-    </row>
-    <row r="18" spans="58:61">
-      <c r="BF18" s="27"/>
-    </row>
-    <row r="22" spans="58:61">
-      <c r="BG22" s="27"/>
-      <c r="BH22" s="27"/>
-      <c r="BI22" s="27"/>
-    </row>
-    <row r="23" spans="58:61">
-      <c r="BG23" s="27"/>
-      <c r="BH23" s="27"/>
-      <c r="BI23" s="27"/>
+      <c r="BY11" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="AN9:AN10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AT9:AT10"/>
-    <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="BE9:BE10"/>
-    <mergeCell ref="BI9:BI10"/>
-    <mergeCell ref="BJ9:BJ10"/>
-    <mergeCell ref="BK9:BK10"/>
-    <mergeCell ref="BO9:BO10"/>
-    <mergeCell ref="BN9:BN10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AL9"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:W8"/>
+    <mergeCell ref="X8:AM8"/>
+    <mergeCell ref="AN8:AP8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:V9"/>
+    <mergeCell ref="X9:X10"/>
     <mergeCell ref="AQ8:AU8"/>
     <mergeCell ref="AV8:AV10"/>
     <mergeCell ref="AW8:AW10"/>
@@ -1896,27 +1911,30 @@
     <mergeCell ref="BG9:BG10"/>
     <mergeCell ref="BH9:BH10"/>
     <mergeCell ref="BU9:BW9"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:W8"/>
-    <mergeCell ref="X8:AM8"/>
-    <mergeCell ref="AN8:AP8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:V9"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AL9"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="AN9:AN10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AU10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="BE9:BE10"/>
+    <mergeCell ref="BI9:BI10"/>
+    <mergeCell ref="BJ9:BJ10"/>
+    <mergeCell ref="BK9:BK10"/>
+    <mergeCell ref="BO9:BO10"/>
+    <mergeCell ref="BN9:BN10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>